<commit_message>
Nearly working, testing still in progress
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/simple_1.xlsx
+++ b/tests/integration_test_files/simple_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C95D93-E3E2-D840-88BB-5551AF005948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3961CEB9-990C-014B-8EE6-8EE126B65A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="3820" windowWidth="33260" windowHeight="19480" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="21900" yWindow="1240" windowWidth="41140" windowHeight="23360" firstSheet="3" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <sheet name="studyDesignProcedures" sheetId="11" r:id="rId12"/>
     <sheet name="studyDesignEncounters" sheetId="12" r:id="rId13"/>
     <sheet name="studyDesignElements" sheetId="13" r:id="rId14"/>
-    <sheet name="configuration" sheetId="10" r:id="rId15"/>
+    <sheet name="studyDesignContent" sheetId="17" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="18" r:id="rId16"/>
+    <sheet name="configuration" sheetId="10" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="629">
   <si>
     <t>Epoch</t>
   </si>
@@ -920,13 +922,1038 @@
   </si>
   <si>
     <t>Only do this if they have two heads</t>
+  </si>
+  <si>
+    <t>sectionTitle</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>PROTOCOL SUMMARY</t>
+  </si>
+  <si>
+    <t>INTRODUCTION</t>
+  </si>
+  <si>
+    <t>TRIAL OBJECTIVES, ENDPOINTS AND ESTIMANDS</t>
+  </si>
+  <si>
+    <t>TRIAL DESIGN</t>
+  </si>
+  <si>
+    <t>TRIAL POPULATION</t>
+  </si>
+  <si>
+    <t>Protocol Synopsis</t>
+  </si>
+  <si>
+    <t>Trial Schema</t>
+  </si>
+  <si>
+    <t>Schedule of Activities</t>
+  </si>
+  <si>
+    <t>Purpose of Trial</t>
+  </si>
+  <si>
+    <t>Summary of Benefits and Risks</t>
+  </si>
+  <si>
+    <t>Description of Trial Design</t>
+  </si>
+  <si>
+    <t>Participant Input into Design</t>
+  </si>
+  <si>
+    <t>Rationale for Trial Design</t>
+  </si>
+  <si>
+    <t>Rationale for Comparator</t>
+  </si>
+  <si>
+    <t>Rationale for Adaptive or Novel Trial Design</t>
+  </si>
+  <si>
+    <t>Other Trial Design Considerations</t>
+  </si>
+  <si>
+    <t>Access to Trial Intervention After End of Trial</t>
+  </si>
+  <si>
+    <t>Start of Trial and End of Trial</t>
+  </si>
+  <si>
+    <t>Selection of Trial Population</t>
+  </si>
+  <si>
+    <t>Rationale for Trial Population</t>
+  </si>
+  <si>
+    <t>Inclusion Criteria</t>
+  </si>
+  <si>
+    <t>Exclusion Criteria</t>
+  </si>
+  <si>
+    <t>Lifestyle Considerations</t>
+  </si>
+  <si>
+    <t>Meals and Dietary Restrictions</t>
+  </si>
+  <si>
+    <t>Caffeine, Alcohol, Tobacco, and Other Habits</t>
+  </si>
+  <si>
+    <t>Physical Activity</t>
+  </si>
+  <si>
+    <t>Other Activity</t>
+  </si>
+  <si>
+    <t>Screen Failures</t>
+  </si>
+  <si>
+    <t>TRIAL INTERVENTION AND CONCOMITANT THERAPY</t>
+  </si>
+  <si>
+    <t>Description of Trial Intervention</t>
+  </si>
+  <si>
+    <t>Rationale for Trial Intervention</t>
+  </si>
+  <si>
+    <t>Dosing and Administration</t>
+  </si>
+  <si>
+    <t>Trial Intervention Dose Modification</t>
+  </si>
+  <si>
+    <t>Treatment of Overdose</t>
+  </si>
+  <si>
+    <t>Preparation, Handling, Storage and Accountability</t>
+  </si>
+  <si>
+    <t>Preparation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>Handling and Storage of Trial Intervention</t>
+  </si>
+  <si>
+    <t>Accountability of Trial Intervention</t>
+  </si>
+  <si>
+    <t>Participant Assignment, Randomisation and Blinding</t>
+  </si>
+  <si>
+    <t>Participant Assignment</t>
+  </si>
+  <si>
+    <t>Randomisation</t>
+  </si>
+  <si>
+    <t>Blinding and Unblinding</t>
+  </si>
+  <si>
+    <t>Trial Intervention Compliance</t>
+  </si>
+  <si>
+    <t>Concomitant Therapy</t>
+  </si>
+  <si>
+    <t>Prohibited Concomitant Therapy</t>
+  </si>
+  <si>
+    <t>Permitted Concomitant Therapy</t>
+  </si>
+  <si>
+    <t>Rescue Therapy</t>
+  </si>
+  <si>
+    <t>Other Therapy</t>
+  </si>
+  <si>
+    <t>DISCONTINUATION OF TRIAL INTERVENTION AND PARTICIP</t>
+  </si>
+  <si>
+    <t>WITHDRAWAL FROM TRIAL</t>
+  </si>
+  <si>
+    <t>Discontinuation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>Criteria for Permanent Discontinuation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>Temporary Discontinuation or Interruption of Trial Intervention</t>
+  </si>
+  <si>
+    <t>Rechallenge</t>
+  </si>
+  <si>
+    <t>Participant Withdrawal from the Trial</t>
+  </si>
+  <si>
+    <t>Lost to Follow-Up</t>
+  </si>
+  <si>
+    <t>Trial Stopping Rules</t>
+  </si>
+  <si>
+    <t>TRIAL ASSESSMENTS AND PROCEDURES</t>
+  </si>
+  <si>
+    <t>Screening/Baseline Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>Efficacy Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>Safety Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>Physical Examination</t>
+  </si>
+  <si>
+    <t>Vital Signs</t>
+  </si>
+  <si>
+    <t>Electrocardiograms</t>
+  </si>
+  <si>
+    <t>Clinical Laboratory Assessments</t>
+  </si>
+  <si>
+    <t>Suicidal Ideation and Behaviour Risk Monitoring</t>
+  </si>
+  <si>
+    <t>Adverse Events and Serious Adverse Events</t>
+  </si>
+  <si>
+    <t>Definitions of AE and SAE</t>
+  </si>
+  <si>
+    <t>Time Period and Frequency for Collecting AE and SAE Information</t>
+  </si>
+  <si>
+    <t>Identifying AEs and SAEs</t>
+  </si>
+  <si>
+    <t>Recording of AEs and SAEs</t>
+  </si>
+  <si>
+    <t>Follow-up of AEs and SAEs</t>
+  </si>
+  <si>
+    <t>Reporting of SAEs</t>
+  </si>
+  <si>
+    <t>Regulatory Reporting Requirements for SAEs</t>
+  </si>
+  <si>
+    <t>Serious and Unexpected Adverse Reaction Reporting</t>
+  </si>
+  <si>
+    <t>Adverse Events of Special Interest</t>
+  </si>
+  <si>
+    <t>Disease-related Events or Outcomes Not Qualifying as AEs or SAEs</t>
+  </si>
+  <si>
+    <t>Pregnancy and Postpartum Information</t>
+  </si>
+  <si>
+    <t>Participants Who Become Pregnant During the Trial</t>
+  </si>
+  <si>
+    <t>Participants Whose Partners Become Pregnant</t>
+  </si>
+  <si>
+    <t>Medical Device Product Complaints for Drug/Device Combination Products</t>
+  </si>
+  <si>
+    <t>Definition of Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>Recording of Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>Time Period and Frequency for Collecting Medical Device Product Complaints .</t>
+  </si>
+  <si>
+    <t>Follow-Up of Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>Regulatory Reporting Requirements for Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>Pharmacokinetics</t>
+  </si>
+  <si>
+    <t>Genetics</t>
+  </si>
+  <si>
+    <t>Biomarkers</t>
+  </si>
+  <si>
+    <t>Immunogenicity Assessments</t>
+  </si>
+  <si>
+    <t>Medical Resource Utilisation and Health Economics</t>
+  </si>
+  <si>
+    <t>STATISTICAL CONSIDERATIONS</t>
+  </si>
+  <si>
+    <t>Analysis Sets</t>
+  </si>
+  <si>
+    <t>Analyses Supporting Primary Objective(s)</t>
+  </si>
+  <si>
+    <t>Statistical Model, Hypothesis, and Method of Analysis</t>
+  </si>
+  <si>
+    <t>Handling of Intercurrent Events of Primary Estimand(s)</t>
+  </si>
+  <si>
+    <t>Handling of Missing Data</t>
+  </si>
+  <si>
+    <t>Sensitivity Analysis</t>
+  </si>
+  <si>
+    <t>Supplementary Analysis</t>
+  </si>
+  <si>
+    <t>Analysis Supporting Secondary Objective(s)</t>
+  </si>
+  <si>
+    <t>Analysis of Exploratory Objective(s)</t>
+  </si>
+  <si>
+    <t>Safety Analyses</t>
+  </si>
+  <si>
+    <t>Other Analyses</t>
+  </si>
+  <si>
+    <t>Interim Analyses</t>
+  </si>
+  <si>
+    <t>Sample Size Determination</t>
+  </si>
+  <si>
+    <t>Protocol Deviations</t>
+  </si>
+  <si>
+    <t>GENERAL CONSIDERATIONS: REGULATORY, ETHICAL, AND TRIAL OVERSIGHT</t>
+  </si>
+  <si>
+    <t>Regulatory and Ethical Considerations</t>
+  </si>
+  <si>
+    <t>Committees</t>
+  </si>
+  <si>
+    <t>Informed Consent Process</t>
+  </si>
+  <si>
+    <t>Data Protection</t>
+  </si>
+  <si>
+    <t>Early Site Closure or Trial Termination</t>
+  </si>
+  <si>
+    <t>GENERAL CONSIDERATIONS: RISK MANAGEMENT AND QUALITY ASSURANCE</t>
+  </si>
+  <si>
+    <t>Quality Tolerance Limits</t>
+  </si>
+  <si>
+    <t>Data Quality Assurance</t>
+  </si>
+  <si>
+    <t>Source Data</t>
+  </si>
+  <si>
+    <t>APPENDIX: ADVERSE EVENTS AND SERIOUS ADVERSE EVENTS - DEFINITIONS, SEVERITY, AND CAUSALITY</t>
+  </si>
+  <si>
+    <t>Further Details and Clarifications on the AE Definition</t>
+  </si>
+  <si>
+    <t>Further Details and Clarifications on the SAE Definition</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Causality</t>
+  </si>
+  <si>
+    <t>APPENDIX: DEFINITIONS AND SUPPORTING OPERATIONAL DETAILS</t>
+  </si>
+  <si>
+    <t>Contraception and Pregnancy Testing</t>
+  </si>
+  <si>
+    <t>Definitions Related to Childbearing Potential</t>
+  </si>
+  <si>
+    <t>Contraception</t>
+  </si>
+  <si>
+    <t>Pregnancy Testing</t>
+  </si>
+  <si>
+    <t>Clinical Laboratory Tests</t>
+  </si>
+  <si>
+    <t>Country/Region-Specific Differences</t>
+  </si>
+  <si>
+    <t>Prior Protocol Amendments</t>
+  </si>
+  <si>
+    <t>APPENDIX: GLOSSARY OF TERMS</t>
+  </si>
+  <si>
+    <t>APPENDIX: REFERENCES</t>
+  </si>
+  <si>
+    <t>DISCONTINUATION OF TRIAL INTERVENTION AND PARTICIPANT WITHDRAWAL FROM TRIAL</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>5.3.1</t>
+  </si>
+  <si>
+    <t>5.3.2</t>
+  </si>
+  <si>
+    <t>5.3.3</t>
+  </si>
+  <si>
+    <t>5.3.4</t>
+  </si>
+  <si>
+    <t>6.3.1</t>
+  </si>
+  <si>
+    <t>6.5.1</t>
+  </si>
+  <si>
+    <t>6.5.2</t>
+  </si>
+  <si>
+    <t>6.5.3</t>
+  </si>
+  <si>
+    <t>6.6.1</t>
+  </si>
+  <si>
+    <t>6.6.2</t>
+  </si>
+  <si>
+    <t>6.6.3</t>
+  </si>
+  <si>
+    <t>6.8.1</t>
+  </si>
+  <si>
+    <t>6.8.2</t>
+  </si>
+  <si>
+    <t>6.8.3</t>
+  </si>
+  <si>
+    <t>6.8.4</t>
+  </si>
+  <si>
+    <t>7.1.1</t>
+  </si>
+  <si>
+    <t>7.1.2</t>
+  </si>
+  <si>
+    <t>7.1.3</t>
+  </si>
+  <si>
+    <t>8.3.1.</t>
+  </si>
+  <si>
+    <t>8.3.2</t>
+  </si>
+  <si>
+    <t>8.3.3</t>
+  </si>
+  <si>
+    <t>8.3.4</t>
+  </si>
+  <si>
+    <t>8.3.5</t>
+  </si>
+  <si>
+    <t>8.4.1.</t>
+  </si>
+  <si>
+    <t>8.4.2</t>
+  </si>
+  <si>
+    <t>8.4.3</t>
+  </si>
+  <si>
+    <t>8.4.4</t>
+  </si>
+  <si>
+    <t>8.4.5</t>
+  </si>
+  <si>
+    <t>8.4.6</t>
+  </si>
+  <si>
+    <t>8.4.7</t>
+  </si>
+  <si>
+    <t>8.4.8</t>
+  </si>
+  <si>
+    <t>8.4.9</t>
+  </si>
+  <si>
+    <t>8.4.10</t>
+  </si>
+  <si>
+    <t>8.5.1</t>
+  </si>
+  <si>
+    <t>8.5.2</t>
+  </si>
+  <si>
+    <t>8.6.1</t>
+  </si>
+  <si>
+    <t>8.6.2</t>
+  </si>
+  <si>
+    <t>8.6.3</t>
+  </si>
+  <si>
+    <t>8.6.4</t>
+  </si>
+  <si>
+    <t>8.6.5</t>
+  </si>
+  <si>
+    <t>9.2.1</t>
+  </si>
+  <si>
+    <t>9.2.2</t>
+  </si>
+  <si>
+    <t>9.2.3</t>
+  </si>
+  <si>
+    <t>9.2.4</t>
+  </si>
+  <si>
+    <t>9.2.5</t>
+  </si>
+  <si>
+    <t>13.1.1</t>
+  </si>
+  <si>
+    <t>13.1.2</t>
+  </si>
+  <si>
+    <t>13.1.3</t>
+  </si>
+  <si>
+    <t>NC1</t>
+  </si>
+  <si>
+    <t>NC2</t>
+  </si>
+  <si>
+    <t>NC3</t>
+  </si>
+  <si>
+    <t>NC4</t>
+  </si>
+  <si>
+    <t>NC5</t>
+  </si>
+  <si>
+    <t>NC6</t>
+  </si>
+  <si>
+    <t>NC7</t>
+  </si>
+  <si>
+    <t>NC8</t>
+  </si>
+  <si>
+    <t>NC9</t>
+  </si>
+  <si>
+    <t>NC10</t>
+  </si>
+  <si>
+    <t>NC11</t>
+  </si>
+  <si>
+    <t>NC12</t>
+  </si>
+  <si>
+    <t>NC13</t>
+  </si>
+  <si>
+    <t>NC14</t>
+  </si>
+  <si>
+    <t>NC15</t>
+  </si>
+  <si>
+    <t>NC16</t>
+  </si>
+  <si>
+    <t>NC17</t>
+  </si>
+  <si>
+    <t>NC18</t>
+  </si>
+  <si>
+    <t>NC19</t>
+  </si>
+  <si>
+    <t>NC20</t>
+  </si>
+  <si>
+    <t>NC21</t>
+  </si>
+  <si>
+    <t>NC22</t>
+  </si>
+  <si>
+    <t>NC23</t>
+  </si>
+  <si>
+    <t>NC24</t>
+  </si>
+  <si>
+    <t>NC25</t>
+  </si>
+  <si>
+    <t>NC26</t>
+  </si>
+  <si>
+    <t>NC27</t>
+  </si>
+  <si>
+    <t>NC28</t>
+  </si>
+  <si>
+    <t>NC29</t>
+  </si>
+  <si>
+    <t>NC30</t>
+  </si>
+  <si>
+    <t>NC31</t>
+  </si>
+  <si>
+    <t>NC32</t>
+  </si>
+  <si>
+    <t>NC33</t>
+  </si>
+  <si>
+    <t>NC34</t>
+  </si>
+  <si>
+    <t>NC35</t>
+  </si>
+  <si>
+    <t>NC36</t>
+  </si>
+  <si>
+    <t>NC37</t>
+  </si>
+  <si>
+    <t>NC38</t>
+  </si>
+  <si>
+    <t>NC39</t>
+  </si>
+  <si>
+    <t>NC40</t>
+  </si>
+  <si>
+    <t>NC41</t>
+  </si>
+  <si>
+    <t>NC42</t>
+  </si>
+  <si>
+    <t>NC43</t>
+  </si>
+  <si>
+    <t>NC44</t>
+  </si>
+  <si>
+    <t>NC45</t>
+  </si>
+  <si>
+    <t>NC46</t>
+  </si>
+  <si>
+    <t>NC47</t>
+  </si>
+  <si>
+    <t>NC48</t>
+  </si>
+  <si>
+    <t>NC49</t>
+  </si>
+  <si>
+    <t>NC50</t>
+  </si>
+  <si>
+    <t>NC51</t>
+  </si>
+  <si>
+    <t>NC52</t>
+  </si>
+  <si>
+    <t>NC53</t>
+  </si>
+  <si>
+    <t>NC54</t>
+  </si>
+  <si>
+    <t>NC55</t>
+  </si>
+  <si>
+    <t>NC56</t>
+  </si>
+  <si>
+    <t>NC57</t>
+  </si>
+  <si>
+    <t>NC58</t>
+  </si>
+  <si>
+    <t>NC59</t>
+  </si>
+  <si>
+    <t>NC60</t>
+  </si>
+  <si>
+    <t>NC61</t>
+  </si>
+  <si>
+    <t>NC62</t>
+  </si>
+  <si>
+    <t>NC63</t>
+  </si>
+  <si>
+    <t>NC64</t>
+  </si>
+  <si>
+    <t>NC65</t>
+  </si>
+  <si>
+    <t>NC66</t>
+  </si>
+  <si>
+    <t>NC67</t>
+  </si>
+  <si>
+    <t>NC68</t>
+  </si>
+  <si>
+    <t>NC69</t>
+  </si>
+  <si>
+    <t>NC70</t>
+  </si>
+  <si>
+    <t>NC71</t>
+  </si>
+  <si>
+    <t>NC72</t>
+  </si>
+  <si>
+    <t>NC73</t>
+  </si>
+  <si>
+    <t>NC74</t>
+  </si>
+  <si>
+    <t>NC75</t>
+  </si>
+  <si>
+    <t>NC76</t>
+  </si>
+  <si>
+    <t>NC77</t>
+  </si>
+  <si>
+    <t>NC78</t>
+  </si>
+  <si>
+    <t>NC79</t>
+  </si>
+  <si>
+    <t>NC80</t>
+  </si>
+  <si>
+    <t>NC81</t>
+  </si>
+  <si>
+    <t>NC82</t>
+  </si>
+  <si>
+    <t>NC83</t>
+  </si>
+  <si>
+    <t>NC84</t>
+  </si>
+  <si>
+    <t>NC85</t>
+  </si>
+  <si>
+    <t>NC86</t>
+  </si>
+  <si>
+    <t>NC87</t>
+  </si>
+  <si>
+    <t>NC88</t>
+  </si>
+  <si>
+    <t>NC89</t>
+  </si>
+  <si>
+    <t>NC90</t>
+  </si>
+  <si>
+    <t>NC91</t>
+  </si>
+  <si>
+    <t>NC92</t>
+  </si>
+  <si>
+    <t>NC93</t>
+  </si>
+  <si>
+    <t>NC94</t>
+  </si>
+  <si>
+    <t>NC95</t>
+  </si>
+  <si>
+    <t>NC96</t>
+  </si>
+  <si>
+    <t>NC97</t>
+  </si>
+  <si>
+    <t>NC98</t>
+  </si>
+  <si>
+    <t>NC99</t>
+  </si>
+  <si>
+    <t>NC100</t>
+  </si>
+  <si>
+    <t>NC101</t>
+  </si>
+  <si>
+    <t>NC102</t>
+  </si>
+  <si>
+    <t>NC103</t>
+  </si>
+  <si>
+    <t>NC104</t>
+  </si>
+  <si>
+    <t>NC105</t>
+  </si>
+  <si>
+    <t>NC106</t>
+  </si>
+  <si>
+    <t>NC107</t>
+  </si>
+  <si>
+    <t>NC108</t>
+  </si>
+  <si>
+    <t>NC109</t>
+  </si>
+  <si>
+    <t>NC110</t>
+  </si>
+  <si>
+    <t>NC111</t>
+  </si>
+  <si>
+    <t>NC112</t>
+  </si>
+  <si>
+    <t>NC113</t>
+  </si>
+  <si>
+    <t>NC114</t>
+  </si>
+  <si>
+    <t>NC115</t>
+  </si>
+  <si>
+    <t>NC116</t>
+  </si>
+  <si>
+    <t>NC117</t>
+  </si>
+  <si>
+    <t>NC118</t>
+  </si>
+  <si>
+    <t>NC119</t>
+  </si>
+  <si>
+    <t>NC120</t>
+  </si>
+  <si>
+    <t>NC121</t>
+  </si>
+  <si>
+    <t>NC122</t>
+  </si>
+  <si>
+    <t>NC123</t>
+  </si>
+  <si>
+    <t>NC124</t>
+  </si>
+  <si>
+    <t>NC125</t>
+  </si>
+  <si>
+    <t>NC126</t>
+  </si>
+  <si>
+    <t>NC127</t>
+  </si>
+  <si>
+    <t>NC128</t>
+  </si>
+  <si>
+    <t>NC129</t>
+  </si>
+  <si>
+    <t>NC130</t>
+  </si>
+  <si>
+    <t>5.5.1</t>
+  </si>
+  <si>
+    <t>5.5.2</t>
+  </si>
+  <si>
+    <t>5.5.3</t>
+  </si>
+  <si>
+    <t>5.5.4</t>
+  </si>
+  <si>
+    <t>8.3.1</t>
+  </si>
+  <si>
+    <t>8.4.1</t>
+  </si>
+  <si>
+    <t>8.1.1</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inclusion criteria are:&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li&gt;1. Something&lt;/li&gt;
+  &lt;li&gt;2. Something else&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Exclusion criteria are:&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li&gt;1. Dont do this&lt;/li&gt;
+  &lt;li&gt;2. And don't do that&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Blinding and unblinding text here please&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>sectionNumber1</t>
+  </si>
+  <si>
+    <t>sectionNumber2</t>
+  </si>
+  <si>
+    <t>sectionNumber3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -964,8 +1991,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -976,6 +2009,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -991,7 +2030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1059,13 +2098,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2284,7 +3334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2564,6 +3614,3435 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
+  <dimension ref="A1:F131"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" style="3" customWidth="1"/>
+    <col min="2" max="4" width="16" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="81.33203125" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>628</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>427</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="E6" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>429</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>430</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="E9" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="E10" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>433</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>424</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>434</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>435</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="C17" s="32">
+        <v>4.3</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="10" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C18" s="32">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="10" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B19" s="32">
+        <v>5</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="C20" s="32">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C21" s="32">
+        <v>5.2</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C22" s="32">
+        <v>5.3</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="C23" s="32">
+        <v>5.4</v>
+      </c>
+      <c r="D23" s="32"/>
+      <c r="E23" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C24" s="32">
+        <v>5.5</v>
+      </c>
+      <c r="D24" s="32"/>
+      <c r="E24" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32" t="s">
+        <v>616</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32" t="s">
+        <v>617</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32" t="s">
+        <v>618</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32" t="s">
+        <v>619</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="C29" s="32">
+        <v>5.6</v>
+      </c>
+      <c r="D29" s="32"/>
+      <c r="E29" s="10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="B30" s="32">
+        <v>6</v>
+      </c>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C31" s="32">
+        <v>6.1</v>
+      </c>
+      <c r="D31" s="32"/>
+      <c r="E31" s="10" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="C32" s="32">
+        <v>6.2</v>
+      </c>
+      <c r="D32" s="32"/>
+      <c r="E32" s="10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="C33" s="32">
+        <v>6.3</v>
+      </c>
+      <c r="D33" s="32"/>
+      <c r="E33" s="10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>442</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="C35" s="32">
+        <v>6.4</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="10" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="C36" s="32">
+        <v>6.5</v>
+      </c>
+      <c r="D36" s="32"/>
+      <c r="E36" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="C40" s="32">
+        <v>6.6</v>
+      </c>
+      <c r="D40" s="32"/>
+      <c r="E40" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>447</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="C44" s="32">
+        <v>6.7</v>
+      </c>
+      <c r="D44" s="32"/>
+      <c r="E44" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="C45" s="32">
+        <v>6.8</v>
+      </c>
+      <c r="D45" s="32"/>
+      <c r="E45" s="10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>449</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>450</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B50" s="32">
+        <v>7</v>
+      </c>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="C51" s="32">
+        <v>7.1</v>
+      </c>
+      <c r="D51" s="32"/>
+      <c r="E51" s="10" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>453</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C55" s="32">
+        <v>7.2</v>
+      </c>
+      <c r="D55" s="32"/>
+      <c r="E55" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="C56" s="32">
+        <v>7.3</v>
+      </c>
+      <c r="D56" s="32"/>
+      <c r="E56" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="C57" s="32">
+        <v>7.4</v>
+      </c>
+      <c r="D57" s="32"/>
+      <c r="E57" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B58" s="32">
+        <v>8</v>
+      </c>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C59" s="32">
+        <v>8.1</v>
+      </c>
+      <c r="D59" s="32"/>
+      <c r="E59" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="C60" s="32">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D60" s="32"/>
+      <c r="E60" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C61" s="32">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D61" s="32"/>
+      <c r="E61" s="10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>620</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>458</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C67" s="32">
+        <v>8.4</v>
+      </c>
+      <c r="D67" s="32"/>
+      <c r="E67" s="10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>621</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="D69" s="32" t="s">
+        <v>462</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="D70" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="D73" s="32" t="s">
+        <v>466</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="D74" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="D75" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="D76" s="32" t="s">
+        <v>469</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="D77" s="32" t="s">
+        <v>470</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="C78" s="32">
+        <v>8.5</v>
+      </c>
+      <c r="D78" s="32"/>
+      <c r="E78" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>471</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="D80" s="32" t="s">
+        <v>472</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C81" s="32">
+        <v>8.6</v>
+      </c>
+      <c r="D81" s="32"/>
+      <c r="E81" s="10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="D82" s="32" t="s">
+        <v>473</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="D83" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="D84" s="32" t="s">
+        <v>475</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D85" s="32" t="s">
+        <v>476</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="D86" s="32" t="s">
+        <v>477</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="C87" s="32">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D87" s="32"/>
+      <c r="E87" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="C88" s="32">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D88" s="32"/>
+      <c r="E88" s="10" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C89" s="32">
+        <v>8.9</v>
+      </c>
+      <c r="D89" s="32"/>
+      <c r="E89" s="10" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="C90" s="32">
+        <v>8.1</v>
+      </c>
+      <c r="D90" s="32"/>
+      <c r="E90" s="10" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="D91" s="32" t="s">
+        <v>622</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="B92" s="32">
+        <v>9</v>
+      </c>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32"/>
+      <c r="E92" s="10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="C93" s="32">
+        <v>9.1</v>
+      </c>
+      <c r="D93" s="32"/>
+      <c r="E93" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="C94" s="32">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D94" s="32"/>
+      <c r="E94" s="10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="D95" s="32" t="s">
+        <v>478</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="D96" s="32" t="s">
+        <v>479</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D97" s="32" t="s">
+        <v>480</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="D98" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D99" s="32" t="s">
+        <v>482</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="C100" s="32">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D100" s="32"/>
+      <c r="E100" s="10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="C101" s="32">
+        <v>9.4</v>
+      </c>
+      <c r="D101" s="32"/>
+      <c r="E101" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="C102" s="32">
+        <v>9.5</v>
+      </c>
+      <c r="D102" s="32"/>
+      <c r="E102" s="10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="C103" s="32">
+        <v>9.6</v>
+      </c>
+      <c r="D103" s="32"/>
+      <c r="E103" s="10" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="C104" s="32">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D104" s="32"/>
+      <c r="E104" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C105" s="32">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D105" s="32"/>
+      <c r="E105" s="10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="C106" s="32">
+        <v>9.9</v>
+      </c>
+      <c r="D106" s="32"/>
+      <c r="E106" s="10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="B107" s="32">
+        <v>10</v>
+      </c>
+      <c r="C107" s="32"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="C108" s="32">
+        <v>10.1</v>
+      </c>
+      <c r="D108" s="32"/>
+      <c r="E108" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C109" s="32">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D109" s="32"/>
+      <c r="E109" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="C110" s="32">
+        <v>10.3</v>
+      </c>
+      <c r="D110" s="32"/>
+      <c r="E110" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="C111" s="32">
+        <v>10.4</v>
+      </c>
+      <c r="D111" s="32"/>
+      <c r="E111" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="C112" s="32">
+        <v>10.5</v>
+      </c>
+      <c r="D112" s="32"/>
+      <c r="E112" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="B113" s="32">
+        <v>11</v>
+      </c>
+      <c r="C113" s="32"/>
+      <c r="D113" s="32"/>
+      <c r="E113" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="C114" s="32">
+        <v>11.1</v>
+      </c>
+      <c r="D114" s="32"/>
+      <c r="E114" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="C115" s="32">
+        <v>11.2</v>
+      </c>
+      <c r="D115" s="32"/>
+      <c r="E115" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="C116" s="32">
+        <v>11.3</v>
+      </c>
+      <c r="D116" s="32"/>
+      <c r="E116" s="10" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B117" s="32">
+        <v>12</v>
+      </c>
+      <c r="C117" s="32"/>
+      <c r="D117" s="32"/>
+      <c r="E117" s="10" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C118" s="32">
+        <v>12.1</v>
+      </c>
+      <c r="D118" s="32"/>
+      <c r="E118" s="10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="C119" s="32">
+        <v>12.2</v>
+      </c>
+      <c r="D119" s="32"/>
+      <c r="E119" s="10" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="C120" s="32">
+        <v>12.3</v>
+      </c>
+      <c r="D120" s="32"/>
+      <c r="E120" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="C121" s="32">
+        <v>12.4</v>
+      </c>
+      <c r="D121" s="32"/>
+      <c r="E121" s="10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="B122" s="32">
+        <v>13</v>
+      </c>
+      <c r="C122" s="32"/>
+      <c r="D122" s="32"/>
+      <c r="E122" s="10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="C123" s="32">
+        <v>13.1</v>
+      </c>
+      <c r="D123" s="32"/>
+      <c r="E123" s="10" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D124" s="32" t="s">
+        <v>483</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="D125" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="D126" s="32" t="s">
+        <v>485</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="C127" s="32">
+        <v>13.2</v>
+      </c>
+      <c r="D127" s="32"/>
+      <c r="E127" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="C128" s="32">
+        <v>13.3</v>
+      </c>
+      <c r="D128" s="32"/>
+      <c r="E128" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C129" s="32">
+        <v>13.4</v>
+      </c>
+      <c r="D129" s="32"/>
+      <c r="E129" s="10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="B130" s="32">
+        <v>14</v>
+      </c>
+      <c r="C130" s="32"/>
+      <c r="D130" s="32"/>
+      <c r="E130" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B131" s="32">
+        <v>15</v>
+      </c>
+      <c r="C131" s="32"/>
+      <c r="D131" s="32"/>
+      <c r="E131" s="10" t="s">
+        <v>422</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0003C67-3768-3A4E-9F90-6843014614B3}">
+  <dimension ref="A1:O131"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:I130"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="29"/>
+    <col min="8" max="8" width="10.83203125" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="29">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>292</v>
+      </c>
+      <c r="O1" s="30" t="str">
+        <f>TEXT(H2,"0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="I2" t="s">
+        <v>297</v>
+      </c>
+      <c r="O2" s="30" t="str">
+        <f>TEXT(H3,"0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
+        <v>1.2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="I3" t="s">
+        <v>298</v>
+      </c>
+      <c r="O3" s="30" t="str">
+        <f>TEXT(H4,"0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="29">
+        <v>1.3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>299</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="I4" t="s">
+        <v>299</v>
+      </c>
+      <c r="O4" s="30" t="str">
+        <f>TEXT(H5,"0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="29">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>293</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="I5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="29">
+        <v>2.1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>300</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="I6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="29">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>301</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="I7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="29">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>294</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="I8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="29">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>295</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="I9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="29">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="I10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="29">
+        <v>0.16737268518518519</v>
+      </c>
+      <c r="B11" t="s">
+        <v>303</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="I11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="29">
+        <v>4.2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="I12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>0.16806712962962964</v>
+      </c>
+      <c r="B13" t="s">
+        <v>305</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="I13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="29">
+        <v>0.1680787037037037</v>
+      </c>
+      <c r="B14" t="s">
+        <v>306</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="I14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>0.16809027777777777</v>
+      </c>
+      <c r="B15" t="s">
+        <v>307</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="I15" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="29">
+        <v>4.3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>308</v>
+      </c>
+      <c r="H16" s="29">
+        <v>4.3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="29">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B17" t="s">
+        <v>309</v>
+      </c>
+      <c r="H17" s="29">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I17" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="29">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>296</v>
+      </c>
+      <c r="H18" s="29">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="29">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B19" t="s">
+        <v>310</v>
+      </c>
+      <c r="H19" s="29">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="29">
+        <v>5.2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>311</v>
+      </c>
+      <c r="H20" s="29">
+        <v>5.2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="29">
+        <v>5.3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>312</v>
+      </c>
+      <c r="H21" s="29">
+        <v>5.3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="29">
+        <v>5.4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>313</v>
+      </c>
+      <c r="H22" s="29">
+        <v>5.4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="29">
+        <v>5.5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>314</v>
+      </c>
+      <c r="H23" s="29">
+        <v>5.5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="29">
+        <v>0.21181712962962962</v>
+      </c>
+      <c r="B24" t="s">
+        <v>315</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="I24" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="29">
+        <v>0.21182870370370369</v>
+      </c>
+      <c r="B25" t="s">
+        <v>316</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="I25" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="29">
+        <v>0.21184027777777778</v>
+      </c>
+      <c r="B26" t="s">
+        <v>317</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="I26" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="29">
+        <v>0.21185185185185185</v>
+      </c>
+      <c r="B27" t="s">
+        <v>318</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="I27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="29">
+        <v>5.6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>319</v>
+      </c>
+      <c r="H28" s="29">
+        <v>5.6</v>
+      </c>
+      <c r="I28" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>320</v>
+      </c>
+      <c r="H29" s="29">
+        <v>6</v>
+      </c>
+      <c r="I29" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="29">
+        <v>6.1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>321</v>
+      </c>
+      <c r="H30" s="29">
+        <v>6.1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="29">
+        <v>6.2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>322</v>
+      </c>
+      <c r="H31" s="29">
+        <v>6.2</v>
+      </c>
+      <c r="I31" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="29">
+        <v>6.3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>323</v>
+      </c>
+      <c r="H32" s="29">
+        <v>6.3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="29">
+        <v>0.25209490740740742</v>
+      </c>
+      <c r="B33" t="s">
+        <v>324</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="I33" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="29">
+        <v>6.4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>325</v>
+      </c>
+      <c r="H34" s="29">
+        <v>6.4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="29">
+        <v>6.5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>326</v>
+      </c>
+      <c r="H35" s="29">
+        <v>6.5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="29">
+        <v>0.2534837962962963</v>
+      </c>
+      <c r="B36" t="s">
+        <v>327</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="I36" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="29">
+        <v>0.25349537037037034</v>
+      </c>
+      <c r="B37" t="s">
+        <v>328</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="I37" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="29">
+        <v>0.25350694444444444</v>
+      </c>
+      <c r="B38" t="s">
+        <v>329</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>445</v>
+      </c>
+      <c r="I38" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="29">
+        <v>6.6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>330</v>
+      </c>
+      <c r="H39" s="29">
+        <v>6.6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="29">
+        <v>0.25417824074074075</v>
+      </c>
+      <c r="B40" t="s">
+        <v>331</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="I40" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="29">
+        <v>0.25418981481481479</v>
+      </c>
+      <c r="B41" t="s">
+        <v>332</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="I41" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="29">
+        <v>0.25420138888888888</v>
+      </c>
+      <c r="B42" t="s">
+        <v>333</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="I42" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="29">
+        <v>6.7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>334</v>
+      </c>
+      <c r="H43" s="29">
+        <v>6.7</v>
+      </c>
+      <c r="I43" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="29">
+        <v>6.8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>335</v>
+      </c>
+      <c r="H44" s="29">
+        <v>6.8</v>
+      </c>
+      <c r="I44" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="29">
+        <v>0.25556712962962963</v>
+      </c>
+      <c r="B45" t="s">
+        <v>336</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>449</v>
+      </c>
+      <c r="I45" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="29">
+        <v>0.25557870370370367</v>
+      </c>
+      <c r="B46" t="s">
+        <v>337</v>
+      </c>
+      <c r="H46" s="29" t="s">
+        <v>450</v>
+      </c>
+      <c r="I46" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="29">
+        <v>0.25559027777777776</v>
+      </c>
+      <c r="B47" t="s">
+        <v>338</v>
+      </c>
+      <c r="H47" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="I47" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="29">
+        <v>0.25560185185185186</v>
+      </c>
+      <c r="B48" t="s">
+        <v>339</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="I48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="29">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>340</v>
+      </c>
+      <c r="H49" s="29">
+        <v>7</v>
+      </c>
+      <c r="I49" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="H50" s="29">
+        <v>7.1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="29">
+        <v>7.1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>342</v>
+      </c>
+      <c r="H51" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="I51" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="29">
+        <v>0.29237268518518517</v>
+      </c>
+      <c r="B52" t="s">
+        <v>343</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="I52" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="29">
+        <v>0.29238425925925926</v>
+      </c>
+      <c r="B53" t="s">
+        <v>344</v>
+      </c>
+      <c r="H53" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="I53" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="29">
+        <v>0.29239583333333335</v>
+      </c>
+      <c r="B54" t="s">
+        <v>345</v>
+      </c>
+      <c r="H54" s="29">
+        <v>7.2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="29">
+        <v>7.2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>346</v>
+      </c>
+      <c r="H55" s="29">
+        <v>7.3</v>
+      </c>
+      <c r="I55" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="29">
+        <v>7.3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>347</v>
+      </c>
+      <c r="H56" s="29">
+        <v>7.4</v>
+      </c>
+      <c r="I56" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="29">
+        <v>7.4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>348</v>
+      </c>
+      <c r="H57" s="29">
+        <v>8</v>
+      </c>
+      <c r="I57" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="29">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>349</v>
+      </c>
+      <c r="H58" s="29">
+        <v>8.1</v>
+      </c>
+      <c r="I58" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="29">
+        <v>8.1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>350</v>
+      </c>
+      <c r="H59" s="29">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I59" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="29">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B60" t="s">
+        <v>351</v>
+      </c>
+      <c r="H60" s="29">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I60" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="29">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B61" t="s">
+        <v>352</v>
+      </c>
+      <c r="H61" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="I61" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="29">
+        <v>0.33542824074074074</v>
+      </c>
+      <c r="B62" t="s">
+        <v>353</v>
+      </c>
+      <c r="H62" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="I62" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="29">
+        <v>0.33543981481481483</v>
+      </c>
+      <c r="B63" t="s">
+        <v>354</v>
+      </c>
+      <c r="H63" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="I63" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="29">
+        <v>0.33545138888888887</v>
+      </c>
+      <c r="B64" t="s">
+        <v>355</v>
+      </c>
+      <c r="H64" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="I64" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="29">
+        <v>0.33546296296296302</v>
+      </c>
+      <c r="B65" t="s">
+        <v>356</v>
+      </c>
+      <c r="H65" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="I65" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="29">
+        <v>0.33547453703703706</v>
+      </c>
+      <c r="B66" t="s">
+        <v>357</v>
+      </c>
+      <c r="H66" s="29">
+        <v>8.4</v>
+      </c>
+      <c r="I66" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="29">
+        <v>8.4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>358</v>
+      </c>
+      <c r="H67" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="I67" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="29">
+        <v>0.33612268518518523</v>
+      </c>
+      <c r="B68" t="s">
+        <v>359</v>
+      </c>
+      <c r="H68" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="I68" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="29">
+        <v>0.33613425925925927</v>
+      </c>
+      <c r="B69" t="s">
+        <v>360</v>
+      </c>
+      <c r="H69" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="I69" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="29">
+        <v>0.33614583333333337</v>
+      </c>
+      <c r="B70" t="s">
+        <v>361</v>
+      </c>
+      <c r="H70" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="I70" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="29">
+        <v>0.3361574074074074</v>
+      </c>
+      <c r="B71" t="s">
+        <v>362</v>
+      </c>
+      <c r="H71" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="I71" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="29">
+        <v>0.3361689814814815</v>
+      </c>
+      <c r="B72" t="s">
+        <v>363</v>
+      </c>
+      <c r="H72" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="I72" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="29">
+        <v>0.33618055555555554</v>
+      </c>
+      <c r="B73" t="s">
+        <v>364</v>
+      </c>
+      <c r="H73" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="I73" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="29">
+        <v>0.33619212962962958</v>
+      </c>
+      <c r="B74" t="s">
+        <v>365</v>
+      </c>
+      <c r="H74" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="I74" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="29">
+        <v>0.33620370370370373</v>
+      </c>
+      <c r="B75" t="s">
+        <v>366</v>
+      </c>
+      <c r="H75" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="I75" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="29">
+        <v>0.33621527777777777</v>
+      </c>
+      <c r="B76" t="s">
+        <v>367</v>
+      </c>
+      <c r="H76" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="I76" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="29">
+        <v>0.33622685185185186</v>
+      </c>
+      <c r="B77" t="s">
+        <v>368</v>
+      </c>
+      <c r="H77" s="29">
+        <v>8.5</v>
+      </c>
+      <c r="I77" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="29">
+        <v>8.5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>369</v>
+      </c>
+      <c r="H78" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="I78" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="29">
+        <v>0.33681712962962962</v>
+      </c>
+      <c r="B79" t="s">
+        <v>370</v>
+      </c>
+      <c r="H79" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="I79" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="29">
+        <v>0.33682870370370371</v>
+      </c>
+      <c r="B80" t="s">
+        <v>371</v>
+      </c>
+      <c r="H80" s="29">
+        <v>8.6</v>
+      </c>
+      <c r="I80" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="29">
+        <v>8.6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>372</v>
+      </c>
+      <c r="H81" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="I81" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="29">
+        <v>0.33751157407407412</v>
+      </c>
+      <c r="B82" t="s">
+        <v>373</v>
+      </c>
+      <c r="H82" s="29" t="s">
+        <v>474</v>
+      </c>
+      <c r="I82" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="29">
+        <v>0.33752314814814816</v>
+      </c>
+      <c r="B83" t="s">
+        <v>374</v>
+      </c>
+      <c r="H83" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="I83" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="29">
+        <v>0.33753472222222225</v>
+      </c>
+      <c r="B84" t="s">
+        <v>375</v>
+      </c>
+      <c r="H84" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="I84" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="29">
+        <v>0.33754629629629629</v>
+      </c>
+      <c r="B85" t="s">
+        <v>376</v>
+      </c>
+      <c r="H85" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="I85" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="29">
+        <v>0.33755787037037038</v>
+      </c>
+      <c r="B86" t="s">
+        <v>377</v>
+      </c>
+      <c r="H86" s="29">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I86" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="29">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="B87" t="s">
+        <v>378</v>
+      </c>
+      <c r="H87" s="29">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I87" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="29">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B88" t="s">
+        <v>379</v>
+      </c>
+      <c r="H88" s="29">
+        <v>8.9</v>
+      </c>
+      <c r="I88" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="29">
+        <v>8.9</v>
+      </c>
+      <c r="B89" t="s">
+        <v>380</v>
+      </c>
+      <c r="H89" s="29">
+        <v>8.1</v>
+      </c>
+      <c r="I89" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="29">
+        <v>8.1</v>
+      </c>
+      <c r="B90" t="s">
+        <v>381</v>
+      </c>
+      <c r="H90" s="29">
+        <v>8.11</v>
+      </c>
+      <c r="I90" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="29">
+        <v>8.11</v>
+      </c>
+      <c r="B91" t="s">
+        <v>382</v>
+      </c>
+      <c r="H91" s="29">
+        <v>9</v>
+      </c>
+      <c r="I91" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="29">
+        <v>9</v>
+      </c>
+      <c r="B92" t="s">
+        <v>383</v>
+      </c>
+      <c r="H92" s="29">
+        <v>9.1</v>
+      </c>
+      <c r="I92" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="29">
+        <v>9.1</v>
+      </c>
+      <c r="B93" t="s">
+        <v>384</v>
+      </c>
+      <c r="H93" s="29">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I93" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="29">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B94" t="s">
+        <v>385</v>
+      </c>
+      <c r="H94" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="I94" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="29">
+        <v>0.37640046296296298</v>
+      </c>
+      <c r="B95" t="s">
+        <v>386</v>
+      </c>
+      <c r="H95" s="29" t="s">
+        <v>479</v>
+      </c>
+      <c r="I95" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="29">
+        <v>0.37641203703703702</v>
+      </c>
+      <c r="B96" t="s">
+        <v>387</v>
+      </c>
+      <c r="H96" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="I96" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="29">
+        <v>0.37642361111111106</v>
+      </c>
+      <c r="B97" t="s">
+        <v>388</v>
+      </c>
+      <c r="H97" s="29" t="s">
+        <v>481</v>
+      </c>
+      <c r="I97" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="29">
+        <v>0.37643518518518521</v>
+      </c>
+      <c r="B98" t="s">
+        <v>389</v>
+      </c>
+      <c r="H98" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="I98" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="29">
+        <v>0.37644675925925924</v>
+      </c>
+      <c r="B99" t="s">
+        <v>390</v>
+      </c>
+      <c r="H99" s="29">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I99" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="29">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B100" t="s">
+        <v>391</v>
+      </c>
+      <c r="H100" s="29">
+        <v>9.4</v>
+      </c>
+      <c r="I100" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="29">
+        <v>9.4</v>
+      </c>
+      <c r="B101" t="s">
+        <v>392</v>
+      </c>
+      <c r="H101" s="29">
+        <v>9.5</v>
+      </c>
+      <c r="I101" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="29">
+        <v>9.5</v>
+      </c>
+      <c r="B102" t="s">
+        <v>393</v>
+      </c>
+      <c r="H102" s="29">
+        <v>9.6</v>
+      </c>
+      <c r="I102" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="29">
+        <v>9.6</v>
+      </c>
+      <c r="B103" t="s">
+        <v>394</v>
+      </c>
+      <c r="H103" s="29">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I103" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="29">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="B104" t="s">
+        <v>395</v>
+      </c>
+      <c r="H104" s="29">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I104" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="29">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B105" t="s">
+        <v>396</v>
+      </c>
+      <c r="H105" s="29">
+        <v>9.9</v>
+      </c>
+      <c r="I105" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" s="29">
+        <v>9.9</v>
+      </c>
+      <c r="B106" t="s">
+        <v>397</v>
+      </c>
+      <c r="H106" s="29">
+        <v>10</v>
+      </c>
+      <c r="I106" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" s="29">
+        <v>10</v>
+      </c>
+      <c r="B107" t="s">
+        <v>398</v>
+      </c>
+      <c r="H107" s="29">
+        <v>10.1</v>
+      </c>
+      <c r="I107" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="29">
+        <v>10.1</v>
+      </c>
+      <c r="B108" t="s">
+        <v>399</v>
+      </c>
+      <c r="H108" s="29">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I108" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="29">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B109" t="s">
+        <v>400</v>
+      </c>
+      <c r="H109" s="29">
+        <v>10.3</v>
+      </c>
+      <c r="I109" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="29">
+        <v>10.3</v>
+      </c>
+      <c r="B110" t="s">
+        <v>401</v>
+      </c>
+      <c r="H110" s="29">
+        <v>10.4</v>
+      </c>
+      <c r="I110" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="29">
+        <v>10.4</v>
+      </c>
+      <c r="B111" t="s">
+        <v>402</v>
+      </c>
+      <c r="H111" s="29">
+        <v>10.5</v>
+      </c>
+      <c r="I111" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" s="29">
+        <v>10.5</v>
+      </c>
+      <c r="B112" t="s">
+        <v>403</v>
+      </c>
+      <c r="H112" s="29">
+        <v>11</v>
+      </c>
+      <c r="I112" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="29">
+        <v>11</v>
+      </c>
+      <c r="B113" t="s">
+        <v>404</v>
+      </c>
+      <c r="H113" s="29">
+        <v>11.1</v>
+      </c>
+      <c r="I113" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="29">
+        <v>11.1</v>
+      </c>
+      <c r="B114" t="s">
+        <v>405</v>
+      </c>
+      <c r="H114" s="29">
+        <v>11.2</v>
+      </c>
+      <c r="I114" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="29">
+        <v>11.2</v>
+      </c>
+      <c r="B115" t="s">
+        <v>406</v>
+      </c>
+      <c r="H115" s="29">
+        <v>11.3</v>
+      </c>
+      <c r="I115" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="29">
+        <v>11.3</v>
+      </c>
+      <c r="B116" t="s">
+        <v>407</v>
+      </c>
+      <c r="H116" s="29">
+        <v>12</v>
+      </c>
+      <c r="I116" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="29">
+        <v>12</v>
+      </c>
+      <c r="B117" t="s">
+        <v>408</v>
+      </c>
+      <c r="H117" s="29">
+        <v>12.1</v>
+      </c>
+      <c r="I117" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="29">
+        <v>12.1</v>
+      </c>
+      <c r="B118" t="s">
+        <v>409</v>
+      </c>
+      <c r="H118" s="29">
+        <v>12.2</v>
+      </c>
+      <c r="I118" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="29">
+        <v>12.2</v>
+      </c>
+      <c r="B119" t="s">
+        <v>410</v>
+      </c>
+      <c r="H119" s="29">
+        <v>12.3</v>
+      </c>
+      <c r="I119" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="29">
+        <v>12.3</v>
+      </c>
+      <c r="B120" t="s">
+        <v>411</v>
+      </c>
+      <c r="H120" s="29">
+        <v>12.4</v>
+      </c>
+      <c r="I120" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="29">
+        <v>12.4</v>
+      </c>
+      <c r="B121" t="s">
+        <v>412</v>
+      </c>
+      <c r="H121" s="29">
+        <v>13</v>
+      </c>
+      <c r="I121" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="29">
+        <v>13</v>
+      </c>
+      <c r="B122" t="s">
+        <v>413</v>
+      </c>
+      <c r="H122" s="29">
+        <v>13.1</v>
+      </c>
+      <c r="I122" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" s="29">
+        <v>13.1</v>
+      </c>
+      <c r="B123" t="s">
+        <v>414</v>
+      </c>
+      <c r="H123" s="29" t="s">
+        <v>483</v>
+      </c>
+      <c r="I123" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="29">
+        <v>0.54237268518518522</v>
+      </c>
+      <c r="B124" t="s">
+        <v>415</v>
+      </c>
+      <c r="H124" s="29" t="s">
+        <v>484</v>
+      </c>
+      <c r="I124" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" s="29">
+        <v>0.54238425925925926</v>
+      </c>
+      <c r="B125" t="s">
+        <v>416</v>
+      </c>
+      <c r="H125" s="29" t="s">
+        <v>485</v>
+      </c>
+      <c r="I125" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="29">
+        <v>0.5423958333333333</v>
+      </c>
+      <c r="B126" t="s">
+        <v>417</v>
+      </c>
+      <c r="H126" s="29">
+        <v>13.2</v>
+      </c>
+      <c r="I126" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" s="29">
+        <v>13.2</v>
+      </c>
+      <c r="B127" t="s">
+        <v>418</v>
+      </c>
+      <c r="H127" s="29">
+        <v>13.3</v>
+      </c>
+      <c r="I127" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="29">
+        <v>13.3</v>
+      </c>
+      <c r="B128" t="s">
+        <v>419</v>
+      </c>
+      <c r="H128" s="29">
+        <v>13.4</v>
+      </c>
+      <c r="I128" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" s="29">
+        <v>13.4</v>
+      </c>
+      <c r="B129" t="s">
+        <v>420</v>
+      </c>
+      <c r="H129" s="29">
+        <v>14</v>
+      </c>
+      <c r="I129" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" s="29">
+        <v>14</v>
+      </c>
+      <c r="B130" t="s">
+        <v>421</v>
+      </c>
+      <c r="H130" s="29">
+        <v>15</v>
+      </c>
+      <c r="I130" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" s="29">
+        <v>15</v>
+      </c>
+      <c r="B131" t="s">
+        <v>422</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2720,34 +7199,34 @@
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
@@ -2867,16 +7346,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3310,7 +7789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8389B3-D1BB-1047-BA06-7E793B938DBA}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First cut cross references
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/simple_1.xlsx
+++ b/tests/integration_test_files/simple_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFCA920F-F1EA-114E-BF82-ADDBDDA1A99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A259DC14-E722-E34F-B590-9D3E47CDAC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42140" yWindow="500" windowWidth="33000" windowHeight="22600" firstSheet="5" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="6" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -28,8 +28,7 @@
     <sheet name="studyDesignEncounters" sheetId="12" r:id="rId13"/>
     <sheet name="studyDesignElements" sheetId="13" r:id="rId14"/>
     <sheet name="studyDesignContent" sheetId="17" r:id="rId15"/>
-    <sheet name="Sheet2" sheetId="18" r:id="rId16"/>
-    <sheet name="configuration" sheetId="10" r:id="rId17"/>
+    <sheet name="configuration" sheetId="10" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="557">
   <si>
     <t>Epoch</t>
   </si>
@@ -1074,12 +1073,6 @@
     <t>Other Therapy</t>
   </si>
   <si>
-    <t>DISCONTINUATION OF TRIAL INTERVENTION AND PARTICIP</t>
-  </si>
-  <si>
-    <t>WITHDRAWAL FROM TRIAL</t>
-  </si>
-  <si>
     <t>Discontinuation of Trial Intervention</t>
   </si>
   <si>
@@ -1368,18 +1361,6 @@
     <t>4.2.3</t>
   </si>
   <si>
-    <t>5.3.1</t>
-  </si>
-  <si>
-    <t>5.3.2</t>
-  </si>
-  <si>
-    <t>5.3.3</t>
-  </si>
-  <si>
-    <t>5.3.4</t>
-  </si>
-  <si>
     <t>6.3.1</t>
   </si>
   <si>
@@ -1422,9 +1403,6 @@
     <t>7.1.3</t>
   </si>
   <si>
-    <t>8.3.1.</t>
-  </si>
-  <si>
     <t>8.3.2</t>
   </si>
   <si>
@@ -1435,9 +1413,6 @@
   </si>
   <si>
     <t>8.3.5</t>
-  </si>
-  <si>
-    <t>8.4.1.</t>
   </si>
   <si>
     <t>8.4.2</t>
@@ -1752,6 +1727,20 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>usdm:ref klass="StudyIdentifier" id="StudyIdentifier_1" attribute="studyIdentifier"/&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1797,9 +1786,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1835,7 +1824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1899,8 +1888,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1914,10 +1901,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3139,7 +3126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3423,7 +3410,7 @@
   <dimension ref="A1:D137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3435,31 +3422,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
-        <v>536</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>496</v>
-      </c>
-      <c r="C1" s="27" t="s">
+      <c r="A1" s="27" t="s">
+        <v>528</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="25" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="10" t="s">
         <v>292</v>
       </c>
+      <c r="D2" s="10" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>297</v>
@@ -3467,7 +3457,7 @@
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>298</v>
@@ -3475,7 +3465,7 @@
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>299</v>
@@ -3483,7 +3473,7 @@
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>293</v>
@@ -3491,7 +3481,7 @@
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>300</v>
@@ -3499,7 +3489,7 @@
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>301</v>
@@ -3507,7 +3497,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>294</v>
@@ -3515,7 +3505,7 @@
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>295</v>
@@ -3523,7 +3513,7 @@
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>302</v>
@@ -3531,1121 +3521,1121 @@
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="B12" s="28"/>
+        <v>422</v>
+      </c>
+      <c r="B12" s="26"/>
       <c r="C12" s="10" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>434</v>
-      </c>
-      <c r="B13" s="28"/>
+        <v>432</v>
+      </c>
+      <c r="B13" s="26"/>
       <c r="C13" s="10" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>435</v>
-      </c>
-      <c r="B14" s="28"/>
+        <v>433</v>
+      </c>
+      <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="B15" s="28"/>
+        <v>434</v>
+      </c>
+      <c r="B15" s="26"/>
       <c r="C15" s="10" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>437</v>
-      </c>
-      <c r="B16" s="28"/>
+        <v>435</v>
+      </c>
+      <c r="B16" s="26"/>
       <c r="C16" s="10" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>519</v>
-      </c>
-      <c r="B17" s="28"/>
+        <v>511</v>
+      </c>
+      <c r="B17" s="26"/>
       <c r="C17" s="10" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>520</v>
-      </c>
-      <c r="B18" s="28"/>
+        <v>512</v>
+      </c>
+      <c r="B18" s="26"/>
       <c r="C18" s="10" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>497</v>
-      </c>
-      <c r="B19" s="28"/>
+        <v>489</v>
+      </c>
+      <c r="B19" s="26"/>
       <c r="C19" s="10" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>521</v>
-      </c>
-      <c r="B20" s="28"/>
+        <v>513</v>
+      </c>
+      <c r="B20" s="26"/>
       <c r="C20" s="10" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>522</v>
-      </c>
-      <c r="B21" s="28"/>
+        <v>514</v>
+      </c>
+      <c r="B21" s="26"/>
       <c r="C21" s="10" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>523</v>
-      </c>
-      <c r="B22" s="28"/>
+        <v>515</v>
+      </c>
+      <c r="B22" s="26"/>
       <c r="C22" s="10" t="s">
         <v>312</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>524</v>
-      </c>
-      <c r="B23" s="28"/>
+        <v>516</v>
+      </c>
+      <c r="B23" s="26"/>
       <c r="C23" s="10" t="s">
         <v>313</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>525</v>
-      </c>
-      <c r="B24" s="28"/>
+        <v>517</v>
+      </c>
+      <c r="B24" s="26"/>
       <c r="C24" s="10" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>486</v>
-      </c>
-      <c r="B25" s="28"/>
+        <v>478</v>
+      </c>
+      <c r="B25" s="26"/>
       <c r="C25" s="10" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>487</v>
-      </c>
-      <c r="B26" s="28"/>
+        <v>479</v>
+      </c>
+      <c r="B26" s="26"/>
       <c r="C26" s="10" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>488</v>
-      </c>
-      <c r="B27" s="28"/>
+        <v>480</v>
+      </c>
+      <c r="B27" s="26"/>
       <c r="C27" s="10" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="B28" s="28"/>
+        <v>481</v>
+      </c>
+      <c r="B28" s="26"/>
       <c r="C28" s="10" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>526</v>
-      </c>
-      <c r="B29" s="28"/>
+        <v>518</v>
+      </c>
+      <c r="B29" s="26"/>
       <c r="C29" s="10" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>498</v>
-      </c>
-      <c r="B30" s="28"/>
+        <v>490</v>
+      </c>
+      <c r="B30" s="26"/>
       <c r="C30" s="10" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="B31" s="28"/>
+        <v>519</v>
+      </c>
+      <c r="B31" s="26"/>
       <c r="C31" s="10" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>528</v>
-      </c>
-      <c r="B32" s="28"/>
+        <v>520</v>
+      </c>
+      <c r="B32" s="26"/>
       <c r="C32" s="10" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>529</v>
-      </c>
-      <c r="B33" s="28"/>
+        <v>521</v>
+      </c>
+      <c r="B33" s="26"/>
       <c r="C33" s="10" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="B34" s="28"/>
+        <v>436</v>
+      </c>
+      <c r="B34" s="26"/>
       <c r="C34" s="10" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>530</v>
-      </c>
-      <c r="B35" s="28"/>
+        <v>522</v>
+      </c>
+      <c r="B35" s="26"/>
       <c r="C35" s="10" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>531</v>
-      </c>
-      <c r="B36" s="28"/>
+        <v>523</v>
+      </c>
+      <c r="B36" s="26"/>
       <c r="C36" s="10" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="B37" s="28"/>
+        <v>437</v>
+      </c>
+      <c r="B37" s="26"/>
       <c r="C37" s="10" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="B38" s="28"/>
+        <v>438</v>
+      </c>
+      <c r="B38" s="26"/>
       <c r="C38" s="10" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="B39" s="28"/>
+        <v>439</v>
+      </c>
+      <c r="B39" s="26"/>
       <c r="C39" s="10" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>532</v>
-      </c>
-      <c r="B40" s="28"/>
+        <v>524</v>
+      </c>
+      <c r="B40" s="26"/>
       <c r="C40" s="10" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="B41" s="28"/>
+        <v>440</v>
+      </c>
+      <c r="B41" s="26"/>
       <c r="C41" s="10" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="B42" s="28"/>
+        <v>441</v>
+      </c>
+      <c r="B42" s="26"/>
       <c r="C42" s="10" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="B43" s="28"/>
+        <v>442</v>
+      </c>
+      <c r="B43" s="26"/>
       <c r="C43" s="10" t="s">
         <v>333</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="B44" s="28"/>
+        <v>525</v>
+      </c>
+      <c r="B44" s="26"/>
       <c r="C44" s="10" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>534</v>
-      </c>
-      <c r="B45" s="28"/>
+        <v>526</v>
+      </c>
+      <c r="B45" s="26"/>
       <c r="C45" s="10" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="B46" s="28"/>
+        <v>443</v>
+      </c>
+      <c r="B46" s="26"/>
       <c r="C46" s="10" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>450</v>
-      </c>
-      <c r="B47" s="28"/>
+        <v>444</v>
+      </c>
+      <c r="B47" s="26"/>
       <c r="C47" s="10" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="B48" s="28"/>
+        <v>445</v>
+      </c>
+      <c r="B48" s="26"/>
       <c r="C48" s="10" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="B49" s="28"/>
+        <v>446</v>
+      </c>
+      <c r="B49" s="26"/>
       <c r="C49" s="10" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>499</v>
-      </c>
-      <c r="B50" s="28"/>
+        <v>491</v>
+      </c>
+      <c r="B50" s="26"/>
       <c r="C50" s="10" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>535</v>
-      </c>
-      <c r="B51" s="28"/>
+        <v>527</v>
+      </c>
+      <c r="B51" s="26"/>
       <c r="C51" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="B52" s="28"/>
+        <v>447</v>
+      </c>
+      <c r="B52" s="26"/>
       <c r="C52" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>454</v>
-      </c>
-      <c r="B53" s="28"/>
+        <v>448</v>
+      </c>
+      <c r="B53" s="26"/>
       <c r="C53" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="B54" s="28"/>
+        <v>449</v>
+      </c>
+      <c r="B54" s="26"/>
       <c r="C54" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="B55" s="28"/>
+        <v>529</v>
+      </c>
+      <c r="B55" s="26"/>
       <c r="C55" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>538</v>
-      </c>
-      <c r="B56" s="28"/>
+        <v>530</v>
+      </c>
+      <c r="B56" s="26"/>
       <c r="C56" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="B57" s="28"/>
+        <v>531</v>
+      </c>
+      <c r="B57" s="26"/>
       <c r="C57" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>500</v>
-      </c>
-      <c r="B58" s="28"/>
+        <v>492</v>
+      </c>
+      <c r="B58" s="26"/>
       <c r="C58" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>540</v>
-      </c>
-      <c r="B59" s="28"/>
+        <v>532</v>
+      </c>
+      <c r="B59" s="26"/>
       <c r="C59" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>541</v>
-      </c>
-      <c r="B60" s="28"/>
+        <v>533</v>
+      </c>
+      <c r="B60" s="26"/>
       <c r="C60" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>542</v>
-      </c>
-      <c r="B61" s="28"/>
+        <v>534</v>
+      </c>
+      <c r="B61" s="26"/>
       <c r="C61" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>490</v>
-      </c>
-      <c r="B62" s="28"/>
+        <v>482</v>
+      </c>
+      <c r="B62" s="26"/>
       <c r="C62" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="B63" s="28"/>
+        <v>450</v>
+      </c>
+      <c r="B63" s="26"/>
       <c r="C63" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="B64" s="28"/>
+        <v>451</v>
+      </c>
+      <c r="B64" s="26"/>
       <c r="C64" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="B65" s="28"/>
+        <v>452</v>
+      </c>
+      <c r="B65" s="26"/>
       <c r="C65" s="10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="B66" s="28"/>
+        <v>453</v>
+      </c>
+      <c r="B66" s="26"/>
       <c r="C66" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="B67" s="28"/>
+        <v>535</v>
+      </c>
+      <c r="B67" s="26"/>
       <c r="C67" s="10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="B68" s="28"/>
+        <v>483</v>
+      </c>
+      <c r="B68" s="26"/>
       <c r="C68" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="B69" s="28"/>
+        <v>454</v>
+      </c>
+      <c r="B69" s="26"/>
       <c r="C69" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="B70" s="28"/>
+        <v>455</v>
+      </c>
+      <c r="B70" s="26"/>
       <c r="C70" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>464</v>
-      </c>
-      <c r="B71" s="28"/>
+        <v>456</v>
+      </c>
+      <c r="B71" s="26"/>
       <c r="C71" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="B72" s="28"/>
+        <v>457</v>
+      </c>
+      <c r="B72" s="26"/>
       <c r="C72" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="B73" s="28"/>
+        <v>458</v>
+      </c>
+      <c r="B73" s="26"/>
       <c r="C73" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="B74" s="28"/>
+        <v>459</v>
+      </c>
+      <c r="B74" s="26"/>
       <c r="C74" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>468</v>
-      </c>
-      <c r="B75" s="28"/>
+        <v>460</v>
+      </c>
+      <c r="B75" s="26"/>
       <c r="C75" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="B76" s="28"/>
+        <v>461</v>
+      </c>
+      <c r="B76" s="26"/>
       <c r="C76" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="B77" s="28"/>
+        <v>462</v>
+      </c>
+      <c r="B77" s="26"/>
       <c r="C77" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="B78" s="28"/>
+        <v>536</v>
+      </c>
+      <c r="B78" s="26"/>
       <c r="C78" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>471</v>
-      </c>
-      <c r="B79" s="28"/>
+        <v>463</v>
+      </c>
+      <c r="B79" s="26"/>
       <c r="C79" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="B80" s="28"/>
+        <v>464</v>
+      </c>
+      <c r="B80" s="26"/>
       <c r="C80" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>545</v>
-      </c>
-      <c r="B81" s="28"/>
+        <v>537</v>
+      </c>
+      <c r="B81" s="26"/>
       <c r="C81" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>473</v>
-      </c>
-      <c r="B82" s="28"/>
+        <v>465</v>
+      </c>
+      <c r="B82" s="26"/>
       <c r="C82" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="B83" s="28"/>
+        <v>466</v>
+      </c>
+      <c r="B83" s="26"/>
       <c r="C83" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>475</v>
-      </c>
-      <c r="B84" s="28"/>
+        <v>467</v>
+      </c>
+      <c r="B84" s="26"/>
       <c r="C84" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>476</v>
-      </c>
-      <c r="B85" s="28"/>
+        <v>468</v>
+      </c>
+      <c r="B85" s="26"/>
       <c r="C85" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>477</v>
-      </c>
-      <c r="B86" s="28"/>
+        <v>469</v>
+      </c>
+      <c r="B86" s="26"/>
       <c r="C86" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>546</v>
-      </c>
-      <c r="B87" s="28"/>
+        <v>538</v>
+      </c>
+      <c r="B87" s="26"/>
       <c r="C87" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>547</v>
-      </c>
-      <c r="B88" s="28"/>
+        <v>539</v>
+      </c>
+      <c r="B88" s="26"/>
       <c r="C88" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>548</v>
-      </c>
-      <c r="B89" s="28"/>
+        <v>540</v>
+      </c>
+      <c r="B89" s="26"/>
       <c r="C89" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>540</v>
-      </c>
-      <c r="B90" s="28"/>
+        <v>532</v>
+      </c>
+      <c r="B90" s="26"/>
       <c r="C90" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>492</v>
-      </c>
-      <c r="B91" s="28"/>
+        <v>484</v>
+      </c>
+      <c r="B91" s="26"/>
       <c r="C91" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>501</v>
-      </c>
-      <c r="B92" s="28"/>
+        <v>493</v>
+      </c>
+      <c r="B92" s="26"/>
       <c r="C92" s="10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="B93" s="28"/>
+        <v>541</v>
+      </c>
+      <c r="B93" s="26"/>
       <c r="C93" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>550</v>
-      </c>
-      <c r="B94" s="28"/>
+        <v>542</v>
+      </c>
+      <c r="B94" s="26"/>
       <c r="C94" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>478</v>
-      </c>
-      <c r="B95" s="28"/>
+        <v>470</v>
+      </c>
+      <c r="B95" s="26"/>
       <c r="C95" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>479</v>
-      </c>
-      <c r="B96" s="28"/>
+        <v>471</v>
+      </c>
+      <c r="B96" s="26"/>
       <c r="C96" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>480</v>
-      </c>
-      <c r="B97" s="28"/>
+        <v>472</v>
+      </c>
+      <c r="B97" s="26"/>
       <c r="C97" s="10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>481</v>
-      </c>
-      <c r="B98" s="28"/>
+        <v>473</v>
+      </c>
+      <c r="B98" s="26"/>
       <c r="C98" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>482</v>
-      </c>
-      <c r="B99" s="28"/>
+        <v>474</v>
+      </c>
+      <c r="B99" s="26"/>
       <c r="C99" s="10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>551</v>
-      </c>
-      <c r="B100" s="28"/>
+        <v>543</v>
+      </c>
+      <c r="B100" s="26"/>
       <c r="C100" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>552</v>
-      </c>
-      <c r="B101" s="28"/>
+        <v>544</v>
+      </c>
+      <c r="B101" s="26"/>
       <c r="C101" s="10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>553</v>
-      </c>
-      <c r="B102" s="28"/>
+        <v>545</v>
+      </c>
+      <c r="B102" s="26"/>
       <c r="C102" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>554</v>
-      </c>
-      <c r="B103" s="28"/>
+        <v>546</v>
+      </c>
+      <c r="B103" s="26"/>
       <c r="C103" s="10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>555</v>
-      </c>
-      <c r="B104" s="28"/>
+        <v>547</v>
+      </c>
+      <c r="B104" s="26"/>
       <c r="C104" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>556</v>
-      </c>
-      <c r="B105" s="28"/>
+        <v>548</v>
+      </c>
+      <c r="B105" s="26"/>
       <c r="C105" s="10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>557</v>
-      </c>
-      <c r="B106" s="28"/>
+        <v>549</v>
+      </c>
+      <c r="B106" s="26"/>
       <c r="C106" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="B107" s="28"/>
+        <v>494</v>
+      </c>
+      <c r="B107" s="26"/>
       <c r="C107" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="B108" s="28"/>
+        <v>550</v>
+      </c>
+      <c r="B108" s="26"/>
       <c r="C108" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>559</v>
-      </c>
-      <c r="B109" s="28"/>
+        <v>551</v>
+      </c>
+      <c r="B109" s="26"/>
       <c r="C109" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>560</v>
-      </c>
-      <c r="B110" s="28"/>
+        <v>552</v>
+      </c>
+      <c r="B110" s="26"/>
       <c r="C110" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>561</v>
-      </c>
-      <c r="B111" s="28"/>
+        <v>553</v>
+      </c>
+      <c r="B111" s="26"/>
       <c r="C111" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>562</v>
-      </c>
-      <c r="B112" s="28"/>
+        <v>554</v>
+      </c>
+      <c r="B112" s="26"/>
       <c r="C112" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>503</v>
-      </c>
-      <c r="B113" s="28"/>
+        <v>495</v>
+      </c>
+      <c r="B113" s="26"/>
       <c r="C113" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>518</v>
-      </c>
-      <c r="B114" s="28"/>
+        <v>510</v>
+      </c>
+      <c r="B114" s="26"/>
       <c r="C114" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="B115" s="28"/>
+        <v>509</v>
+      </c>
+      <c r="B115" s="26"/>
       <c r="C115" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>516</v>
-      </c>
-      <c r="B116" s="28"/>
+        <v>508</v>
+      </c>
+      <c r="B116" s="26"/>
       <c r="C116" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>504</v>
-      </c>
-      <c r="B117" s="28"/>
+        <v>496</v>
+      </c>
+      <c r="B117" s="26"/>
       <c r="C117" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>515</v>
-      </c>
-      <c r="B118" s="28"/>
+        <v>507</v>
+      </c>
+      <c r="B118" s="26"/>
       <c r="C118" s="10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>514</v>
-      </c>
-      <c r="B119" s="28"/>
+        <v>506</v>
+      </c>
+      <c r="B119" s="26"/>
       <c r="C119" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>513</v>
-      </c>
-      <c r="B120" s="28"/>
+        <v>505</v>
+      </c>
+      <c r="B120" s="26"/>
       <c r="C120" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>512</v>
-      </c>
-      <c r="B121" s="28"/>
+        <v>504</v>
+      </c>
+      <c r="B121" s="26"/>
       <c r="C121" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="B122" s="28"/>
+        <v>497</v>
+      </c>
+      <c r="B122" s="26"/>
       <c r="C122" s="10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>511</v>
-      </c>
-      <c r="B123" s="28"/>
+        <v>503</v>
+      </c>
+      <c r="B123" s="26"/>
       <c r="C123" s="10" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
-        <v>483</v>
-      </c>
-      <c r="B124" s="28"/>
+        <v>475</v>
+      </c>
+      <c r="B124" s="26"/>
       <c r="C124" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="B125" s="28"/>
+        <v>476</v>
+      </c>
+      <c r="B125" s="26"/>
       <c r="C125" s="10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>485</v>
-      </c>
-      <c r="B126" s="28"/>
+        <v>477</v>
+      </c>
+      <c r="B126" s="26"/>
       <c r="C126" s="10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>510</v>
-      </c>
-      <c r="B127" s="28"/>
+        <v>502</v>
+      </c>
+      <c r="B127" s="26"/>
       <c r="C127" s="10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>509</v>
-      </c>
-      <c r="B128" s="28"/>
+        <v>501</v>
+      </c>
+      <c r="B128" s="26"/>
       <c r="C128" s="10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>508</v>
-      </c>
-      <c r="B129" s="28"/>
+        <v>500</v>
+      </c>
+      <c r="B129" s="26"/>
       <c r="C129" s="10" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>506</v>
-      </c>
-      <c r="B130" s="28"/>
+        <v>498</v>
+      </c>
+      <c r="B130" s="26"/>
       <c r="C130" s="10" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="B131" s="28"/>
+        <v>499</v>
+      </c>
+      <c r="B131" s="26"/>
       <c r="C131" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -4655,1867 +4645,6 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0003C67-3768-3A4E-9F90-6843014614B3}">
-  <dimension ref="A1:O131"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I130"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="25"/>
-    <col min="8" max="8" width="10.83203125" style="25"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="25">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>292</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>292</v>
-      </c>
-      <c r="O1" s="26" t="str">
-        <f>TEXT(H2,"0")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A2" s="25">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="I2" t="s">
-        <v>297</v>
-      </c>
-      <c r="O2" s="26" t="str">
-        <f>TEXT(H3,"0")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="25">
-        <v>1.2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>426</v>
-      </c>
-      <c r="I3" t="s">
-        <v>298</v>
-      </c>
-      <c r="O3" s="26" t="str">
-        <f>TEXT(H4,"0")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="25">
-        <v>1.3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>299</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>427</v>
-      </c>
-      <c r="I4" t="s">
-        <v>299</v>
-      </c>
-      <c r="O4" s="26" t="str">
-        <f>TEXT(H5,"0")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="25">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>293</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>428</v>
-      </c>
-      <c r="I5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="25">
-        <v>2.1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>300</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>429</v>
-      </c>
-      <c r="I6" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="25">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B7" t="s">
-        <v>301</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>430</v>
-      </c>
-      <c r="I7" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="25">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>294</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>431</v>
-      </c>
-      <c r="I8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="25">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>295</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>432</v>
-      </c>
-      <c r="I9" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="25">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B10" t="s">
-        <v>302</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>433</v>
-      </c>
-      <c r="I10" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="25">
-        <v>0.16737268518518519</v>
-      </c>
-      <c r="B11" t="s">
-        <v>303</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>424</v>
-      </c>
-      <c r="I11" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="25">
-        <v>4.2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>304</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="I12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="25">
-        <v>0.16806712962962964</v>
-      </c>
-      <c r="B13" t="s">
-        <v>305</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="I13" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="25">
-        <v>0.1680787037037037</v>
-      </c>
-      <c r="B14" t="s">
-        <v>306</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="I14" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="25">
-        <v>0.16809027777777777</v>
-      </c>
-      <c r="B15" t="s">
-        <v>307</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>437</v>
-      </c>
-      <c r="I15" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="25">
-        <v>4.3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>308</v>
-      </c>
-      <c r="H16" s="25">
-        <v>4.3</v>
-      </c>
-      <c r="I16" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="25">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B17" t="s">
-        <v>309</v>
-      </c>
-      <c r="H17" s="25">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I17" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="25">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>296</v>
-      </c>
-      <c r="H18" s="25">
-        <v>5</v>
-      </c>
-      <c r="I18" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="25">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B19" t="s">
-        <v>310</v>
-      </c>
-      <c r="H19" s="25">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="I19" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="25">
-        <v>5.2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>311</v>
-      </c>
-      <c r="H20" s="25">
-        <v>5.2</v>
-      </c>
-      <c r="I20" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="25">
-        <v>5.3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>312</v>
-      </c>
-      <c r="H21" s="25">
-        <v>5.3</v>
-      </c>
-      <c r="I21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="25">
-        <v>5.4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>313</v>
-      </c>
-      <c r="H22" s="25">
-        <v>5.4</v>
-      </c>
-      <c r="I22" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="25">
-        <v>5.5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>314</v>
-      </c>
-      <c r="H23" s="25">
-        <v>5.5</v>
-      </c>
-      <c r="I23" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="25">
-        <v>0.21181712962962962</v>
-      </c>
-      <c r="B24" t="s">
-        <v>315</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>438</v>
-      </c>
-      <c r="I24" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="25">
-        <v>0.21182870370370369</v>
-      </c>
-      <c r="B25" t="s">
-        <v>316</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>439</v>
-      </c>
-      <c r="I25" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="25">
-        <v>0.21184027777777778</v>
-      </c>
-      <c r="B26" t="s">
-        <v>317</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>440</v>
-      </c>
-      <c r="I26" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="25">
-        <v>0.21185185185185185</v>
-      </c>
-      <c r="B27" t="s">
-        <v>318</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>441</v>
-      </c>
-      <c r="I27" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="25">
-        <v>5.6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>319</v>
-      </c>
-      <c r="H28" s="25">
-        <v>5.6</v>
-      </c>
-      <c r="I28" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="25">
-        <v>6</v>
-      </c>
-      <c r="B29" t="s">
-        <v>320</v>
-      </c>
-      <c r="H29" s="25">
-        <v>6</v>
-      </c>
-      <c r="I29" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="25">
-        <v>6.1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>321</v>
-      </c>
-      <c r="H30" s="25">
-        <v>6.1</v>
-      </c>
-      <c r="I30" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="25">
-        <v>6.2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>322</v>
-      </c>
-      <c r="H31" s="25">
-        <v>6.2</v>
-      </c>
-      <c r="I31" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="25">
-        <v>6.3</v>
-      </c>
-      <c r="B32" t="s">
-        <v>323</v>
-      </c>
-      <c r="H32" s="25">
-        <v>6.3</v>
-      </c>
-      <c r="I32" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="25">
-        <v>0.25209490740740742</v>
-      </c>
-      <c r="B33" t="s">
-        <v>324</v>
-      </c>
-      <c r="H33" s="25" t="s">
-        <v>442</v>
-      </c>
-      <c r="I33" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="25">
-        <v>6.4</v>
-      </c>
-      <c r="B34" t="s">
-        <v>325</v>
-      </c>
-      <c r="H34" s="25">
-        <v>6.4</v>
-      </c>
-      <c r="I34" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="25">
-        <v>6.5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>326</v>
-      </c>
-      <c r="H35" s="25">
-        <v>6.5</v>
-      </c>
-      <c r="I35" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="25">
-        <v>0.2534837962962963</v>
-      </c>
-      <c r="B36" t="s">
-        <v>327</v>
-      </c>
-      <c r="H36" s="25" t="s">
-        <v>443</v>
-      </c>
-      <c r="I36" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="25">
-        <v>0.25349537037037034</v>
-      </c>
-      <c r="B37" t="s">
-        <v>328</v>
-      </c>
-      <c r="H37" s="25" t="s">
-        <v>444</v>
-      </c>
-      <c r="I37" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="25">
-        <v>0.25350694444444444</v>
-      </c>
-      <c r="B38" t="s">
-        <v>329</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>445</v>
-      </c>
-      <c r="I38" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="25">
-        <v>6.6</v>
-      </c>
-      <c r="B39" t="s">
-        <v>330</v>
-      </c>
-      <c r="H39" s="25">
-        <v>6.6</v>
-      </c>
-      <c r="I39" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="25">
-        <v>0.25417824074074075</v>
-      </c>
-      <c r="B40" t="s">
-        <v>331</v>
-      </c>
-      <c r="H40" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="I40" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="25">
-        <v>0.25418981481481479</v>
-      </c>
-      <c r="B41" t="s">
-        <v>332</v>
-      </c>
-      <c r="H41" s="25" t="s">
-        <v>447</v>
-      </c>
-      <c r="I41" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="25">
-        <v>0.25420138888888888</v>
-      </c>
-      <c r="B42" t="s">
-        <v>333</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>448</v>
-      </c>
-      <c r="I42" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="25">
-        <v>6.7</v>
-      </c>
-      <c r="B43" t="s">
-        <v>334</v>
-      </c>
-      <c r="H43" s="25">
-        <v>6.7</v>
-      </c>
-      <c r="I43" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="25">
-        <v>6.8</v>
-      </c>
-      <c r="B44" t="s">
-        <v>335</v>
-      </c>
-      <c r="H44" s="25">
-        <v>6.8</v>
-      </c>
-      <c r="I44" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="25">
-        <v>0.25556712962962963</v>
-      </c>
-      <c r="B45" t="s">
-        <v>336</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>449</v>
-      </c>
-      <c r="I45" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="25">
-        <v>0.25557870370370367</v>
-      </c>
-      <c r="B46" t="s">
-        <v>337</v>
-      </c>
-      <c r="H46" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="I46" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="25">
-        <v>0.25559027777777776</v>
-      </c>
-      <c r="B47" t="s">
-        <v>338</v>
-      </c>
-      <c r="H47" s="25" t="s">
-        <v>451</v>
-      </c>
-      <c r="I47" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="25">
-        <v>0.25560185185185186</v>
-      </c>
-      <c r="B48" t="s">
-        <v>339</v>
-      </c>
-      <c r="H48" s="25" t="s">
-        <v>452</v>
-      </c>
-      <c r="I48" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="25">
-        <v>7</v>
-      </c>
-      <c r="B49" t="s">
-        <v>340</v>
-      </c>
-      <c r="H49" s="25">
-        <v>7</v>
-      </c>
-      <c r="I49" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="25" t="s">
-        <v>341</v>
-      </c>
-      <c r="H50" s="25">
-        <v>7.1</v>
-      </c>
-      <c r="I50" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="25">
-        <v>7.1</v>
-      </c>
-      <c r="B51" t="s">
-        <v>342</v>
-      </c>
-      <c r="H51" s="25" t="s">
-        <v>453</v>
-      </c>
-      <c r="I51" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="25">
-        <v>0.29237268518518517</v>
-      </c>
-      <c r="B52" t="s">
-        <v>343</v>
-      </c>
-      <c r="H52" s="25" t="s">
-        <v>454</v>
-      </c>
-      <c r="I52" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="25">
-        <v>0.29238425925925926</v>
-      </c>
-      <c r="B53" t="s">
-        <v>344</v>
-      </c>
-      <c r="H53" s="25" t="s">
-        <v>455</v>
-      </c>
-      <c r="I53" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="25">
-        <v>0.29239583333333335</v>
-      </c>
-      <c r="B54" t="s">
-        <v>345</v>
-      </c>
-      <c r="H54" s="25">
-        <v>7.2</v>
-      </c>
-      <c r="I54" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="25">
-        <v>7.2</v>
-      </c>
-      <c r="B55" t="s">
-        <v>346</v>
-      </c>
-      <c r="H55" s="25">
-        <v>7.3</v>
-      </c>
-      <c r="I55" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="25">
-        <v>7.3</v>
-      </c>
-      <c r="B56" t="s">
-        <v>347</v>
-      </c>
-      <c r="H56" s="25">
-        <v>7.4</v>
-      </c>
-      <c r="I56" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="25">
-        <v>7.4</v>
-      </c>
-      <c r="B57" t="s">
-        <v>348</v>
-      </c>
-      <c r="H57" s="25">
-        <v>8</v>
-      </c>
-      <c r="I57" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="25">
-        <v>8</v>
-      </c>
-      <c r="B58" t="s">
-        <v>349</v>
-      </c>
-      <c r="H58" s="25">
-        <v>8.1</v>
-      </c>
-      <c r="I58" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="25">
-        <v>8.1</v>
-      </c>
-      <c r="B59" t="s">
-        <v>350</v>
-      </c>
-      <c r="H59" s="25">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I59" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="25">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B60" t="s">
-        <v>351</v>
-      </c>
-      <c r="H60" s="25">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I60" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="25">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="B61" t="s">
-        <v>352</v>
-      </c>
-      <c r="H61" s="25" t="s">
-        <v>456</v>
-      </c>
-      <c r="I61" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="25">
-        <v>0.33542824074074074</v>
-      </c>
-      <c r="B62" t="s">
-        <v>353</v>
-      </c>
-      <c r="H62" s="25" t="s">
-        <v>457</v>
-      </c>
-      <c r="I62" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="25">
-        <v>0.33543981481481483</v>
-      </c>
-      <c r="B63" t="s">
-        <v>354</v>
-      </c>
-      <c r="H63" s="25" t="s">
-        <v>458</v>
-      </c>
-      <c r="I63" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="25">
-        <v>0.33545138888888887</v>
-      </c>
-      <c r="B64" t="s">
-        <v>355</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>459</v>
-      </c>
-      <c r="I64" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="25">
-        <v>0.33546296296296302</v>
-      </c>
-      <c r="B65" t="s">
-        <v>356</v>
-      </c>
-      <c r="H65" s="25" t="s">
-        <v>460</v>
-      </c>
-      <c r="I65" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="25">
-        <v>0.33547453703703706</v>
-      </c>
-      <c r="B66" t="s">
-        <v>357</v>
-      </c>
-      <c r="H66" s="25">
-        <v>8.4</v>
-      </c>
-      <c r="I66" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="25">
-        <v>8.4</v>
-      </c>
-      <c r="B67" t="s">
-        <v>358</v>
-      </c>
-      <c r="H67" s="25" t="s">
-        <v>461</v>
-      </c>
-      <c r="I67" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="25">
-        <v>0.33612268518518523</v>
-      </c>
-      <c r="B68" t="s">
-        <v>359</v>
-      </c>
-      <c r="H68" s="25" t="s">
-        <v>462</v>
-      </c>
-      <c r="I68" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="25">
-        <v>0.33613425925925927</v>
-      </c>
-      <c r="B69" t="s">
-        <v>360</v>
-      </c>
-      <c r="H69" s="25" t="s">
-        <v>463</v>
-      </c>
-      <c r="I69" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="25">
-        <v>0.33614583333333337</v>
-      </c>
-      <c r="B70" t="s">
-        <v>361</v>
-      </c>
-      <c r="H70" s="25" t="s">
-        <v>464</v>
-      </c>
-      <c r="I70" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="25">
-        <v>0.3361574074074074</v>
-      </c>
-      <c r="B71" t="s">
-        <v>362</v>
-      </c>
-      <c r="H71" s="25" t="s">
-        <v>465</v>
-      </c>
-      <c r="I71" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="25">
-        <v>0.3361689814814815</v>
-      </c>
-      <c r="B72" t="s">
-        <v>363</v>
-      </c>
-      <c r="H72" s="25" t="s">
-        <v>466</v>
-      </c>
-      <c r="I72" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="25">
-        <v>0.33618055555555554</v>
-      </c>
-      <c r="B73" t="s">
-        <v>364</v>
-      </c>
-      <c r="H73" s="25" t="s">
-        <v>467</v>
-      </c>
-      <c r="I73" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="25">
-        <v>0.33619212962962958</v>
-      </c>
-      <c r="B74" t="s">
-        <v>365</v>
-      </c>
-      <c r="H74" s="25" t="s">
-        <v>468</v>
-      </c>
-      <c r="I74" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="25">
-        <v>0.33620370370370373</v>
-      </c>
-      <c r="B75" t="s">
-        <v>366</v>
-      </c>
-      <c r="H75" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="I75" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="25">
-        <v>0.33621527777777777</v>
-      </c>
-      <c r="B76" t="s">
-        <v>367</v>
-      </c>
-      <c r="H76" s="25" t="s">
-        <v>470</v>
-      </c>
-      <c r="I76" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="25">
-        <v>0.33622685185185186</v>
-      </c>
-      <c r="B77" t="s">
-        <v>368</v>
-      </c>
-      <c r="H77" s="25">
-        <v>8.5</v>
-      </c>
-      <c r="I77" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="25">
-        <v>8.5</v>
-      </c>
-      <c r="B78" t="s">
-        <v>369</v>
-      </c>
-      <c r="H78" s="25" t="s">
-        <v>471</v>
-      </c>
-      <c r="I78" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="25">
-        <v>0.33681712962962962</v>
-      </c>
-      <c r="B79" t="s">
-        <v>370</v>
-      </c>
-      <c r="H79" s="25" t="s">
-        <v>472</v>
-      </c>
-      <c r="I79" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="25">
-        <v>0.33682870370370371</v>
-      </c>
-      <c r="B80" t="s">
-        <v>371</v>
-      </c>
-      <c r="H80" s="25">
-        <v>8.6</v>
-      </c>
-      <c r="I80" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="25">
-        <v>8.6</v>
-      </c>
-      <c r="B81" t="s">
-        <v>372</v>
-      </c>
-      <c r="H81" s="25" t="s">
-        <v>473</v>
-      </c>
-      <c r="I81" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="25">
-        <v>0.33751157407407412</v>
-      </c>
-      <c r="B82" t="s">
-        <v>373</v>
-      </c>
-      <c r="H82" s="25" t="s">
-        <v>474</v>
-      </c>
-      <c r="I82" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="25">
-        <v>0.33752314814814816</v>
-      </c>
-      <c r="B83" t="s">
-        <v>374</v>
-      </c>
-      <c r="H83" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="I83" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="25">
-        <v>0.33753472222222225</v>
-      </c>
-      <c r="B84" t="s">
-        <v>375</v>
-      </c>
-      <c r="H84" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="I84" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="25">
-        <v>0.33754629629629629</v>
-      </c>
-      <c r="B85" t="s">
-        <v>376</v>
-      </c>
-      <c r="H85" s="25" t="s">
-        <v>477</v>
-      </c>
-      <c r="I85" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="25">
-        <v>0.33755787037037038</v>
-      </c>
-      <c r="B86" t="s">
-        <v>377</v>
-      </c>
-      <c r="H86" s="25">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="I86" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="25">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="B87" t="s">
-        <v>378</v>
-      </c>
-      <c r="H87" s="25">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="I87" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="25">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="B88" t="s">
-        <v>379</v>
-      </c>
-      <c r="H88" s="25">
-        <v>8.9</v>
-      </c>
-      <c r="I88" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="25">
-        <v>8.9</v>
-      </c>
-      <c r="B89" t="s">
-        <v>380</v>
-      </c>
-      <c r="H89" s="25">
-        <v>8.1</v>
-      </c>
-      <c r="I89" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="25">
-        <v>8.1</v>
-      </c>
-      <c r="B90" t="s">
-        <v>381</v>
-      </c>
-      <c r="H90" s="25">
-        <v>8.11</v>
-      </c>
-      <c r="I90" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="25">
-        <v>8.11</v>
-      </c>
-      <c r="B91" t="s">
-        <v>382</v>
-      </c>
-      <c r="H91" s="25">
-        <v>9</v>
-      </c>
-      <c r="I91" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" s="25">
-        <v>9</v>
-      </c>
-      <c r="B92" t="s">
-        <v>383</v>
-      </c>
-      <c r="H92" s="25">
-        <v>9.1</v>
-      </c>
-      <c r="I92" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="25">
-        <v>9.1</v>
-      </c>
-      <c r="B93" t="s">
-        <v>384</v>
-      </c>
-      <c r="H93" s="25">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="I93" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="25">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B94" t="s">
-        <v>385</v>
-      </c>
-      <c r="H94" s="25" t="s">
-        <v>478</v>
-      </c>
-      <c r="I94" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="25">
-        <v>0.37640046296296298</v>
-      </c>
-      <c r="B95" t="s">
-        <v>386</v>
-      </c>
-      <c r="H95" s="25" t="s">
-        <v>479</v>
-      </c>
-      <c r="I95" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="25">
-        <v>0.37641203703703702</v>
-      </c>
-      <c r="B96" t="s">
-        <v>387</v>
-      </c>
-      <c r="H96" s="25" t="s">
-        <v>480</v>
-      </c>
-      <c r="I96" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="25">
-        <v>0.37642361111111106</v>
-      </c>
-      <c r="B97" t="s">
-        <v>388</v>
-      </c>
-      <c r="H97" s="25" t="s">
-        <v>481</v>
-      </c>
-      <c r="I97" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" s="25">
-        <v>0.37643518518518521</v>
-      </c>
-      <c r="B98" t="s">
-        <v>389</v>
-      </c>
-      <c r="H98" s="25" t="s">
-        <v>482</v>
-      </c>
-      <c r="I98" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" s="25">
-        <v>0.37644675925925924</v>
-      </c>
-      <c r="B99" t="s">
-        <v>390</v>
-      </c>
-      <c r="H99" s="25">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="I99" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A100" s="25">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="B100" t="s">
-        <v>391</v>
-      </c>
-      <c r="H100" s="25">
-        <v>9.4</v>
-      </c>
-      <c r="I100" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="25">
-        <v>9.4</v>
-      </c>
-      <c r="B101" t="s">
-        <v>392</v>
-      </c>
-      <c r="H101" s="25">
-        <v>9.5</v>
-      </c>
-      <c r="I101" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="25">
-        <v>9.5</v>
-      </c>
-      <c r="B102" t="s">
-        <v>393</v>
-      </c>
-      <c r="H102" s="25">
-        <v>9.6</v>
-      </c>
-      <c r="I102" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103" s="25">
-        <v>9.6</v>
-      </c>
-      <c r="B103" t="s">
-        <v>394</v>
-      </c>
-      <c r="H103" s="25">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="I103" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A104" s="25">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="B104" t="s">
-        <v>395</v>
-      </c>
-      <c r="H104" s="25">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="I104" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A105" s="25">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="B105" t="s">
-        <v>396</v>
-      </c>
-      <c r="H105" s="25">
-        <v>9.9</v>
-      </c>
-      <c r="I105" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A106" s="25">
-        <v>9.9</v>
-      </c>
-      <c r="B106" t="s">
-        <v>397</v>
-      </c>
-      <c r="H106" s="25">
-        <v>10</v>
-      </c>
-      <c r="I106" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" s="25">
-        <v>10</v>
-      </c>
-      <c r="B107" t="s">
-        <v>398</v>
-      </c>
-      <c r="H107" s="25">
-        <v>10.1</v>
-      </c>
-      <c r="I107" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" s="25">
-        <v>10.1</v>
-      </c>
-      <c r="B108" t="s">
-        <v>399</v>
-      </c>
-      <c r="H108" s="25">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="I108" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A109" s="25">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="B109" t="s">
-        <v>400</v>
-      </c>
-      <c r="H109" s="25">
-        <v>10.3</v>
-      </c>
-      <c r="I109" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="25">
-        <v>10.3</v>
-      </c>
-      <c r="B110" t="s">
-        <v>401</v>
-      </c>
-      <c r="H110" s="25">
-        <v>10.4</v>
-      </c>
-      <c r="I110" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" s="25">
-        <v>10.4</v>
-      </c>
-      <c r="B111" t="s">
-        <v>402</v>
-      </c>
-      <c r="H111" s="25">
-        <v>10.5</v>
-      </c>
-      <c r="I111" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A112" s="25">
-        <v>10.5</v>
-      </c>
-      <c r="B112" t="s">
-        <v>403</v>
-      </c>
-      <c r="H112" s="25">
-        <v>11</v>
-      </c>
-      <c r="I112" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="25">
-        <v>11</v>
-      </c>
-      <c r="B113" t="s">
-        <v>404</v>
-      </c>
-      <c r="H113" s="25">
-        <v>11.1</v>
-      </c>
-      <c r="I113" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="25">
-        <v>11.1</v>
-      </c>
-      <c r="B114" t="s">
-        <v>405</v>
-      </c>
-      <c r="H114" s="25">
-        <v>11.2</v>
-      </c>
-      <c r="I114" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" s="25">
-        <v>11.2</v>
-      </c>
-      <c r="B115" t="s">
-        <v>406</v>
-      </c>
-      <c r="H115" s="25">
-        <v>11.3</v>
-      </c>
-      <c r="I115" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A116" s="25">
-        <v>11.3</v>
-      </c>
-      <c r="B116" t="s">
-        <v>407</v>
-      </c>
-      <c r="H116" s="25">
-        <v>12</v>
-      </c>
-      <c r="I116" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" s="25">
-        <v>12</v>
-      </c>
-      <c r="B117" t="s">
-        <v>408</v>
-      </c>
-      <c r="H117" s="25">
-        <v>12.1</v>
-      </c>
-      <c r="I117" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A118" s="25">
-        <v>12.1</v>
-      </c>
-      <c r="B118" t="s">
-        <v>409</v>
-      </c>
-      <c r="H118" s="25">
-        <v>12.2</v>
-      </c>
-      <c r="I118" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="25">
-        <v>12.2</v>
-      </c>
-      <c r="B119" t="s">
-        <v>410</v>
-      </c>
-      <c r="H119" s="25">
-        <v>12.3</v>
-      </c>
-      <c r="I119" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="25">
-        <v>12.3</v>
-      </c>
-      <c r="B120" t="s">
-        <v>411</v>
-      </c>
-      <c r="H120" s="25">
-        <v>12.4</v>
-      </c>
-      <c r="I120" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A121" s="25">
-        <v>12.4</v>
-      </c>
-      <c r="B121" t="s">
-        <v>412</v>
-      </c>
-      <c r="H121" s="25">
-        <v>13</v>
-      </c>
-      <c r="I121" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A122" s="25">
-        <v>13</v>
-      </c>
-      <c r="B122" t="s">
-        <v>413</v>
-      </c>
-      <c r="H122" s="25">
-        <v>13.1</v>
-      </c>
-      <c r="I122" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="25">
-        <v>13.1</v>
-      </c>
-      <c r="B123" t="s">
-        <v>414</v>
-      </c>
-      <c r="H123" s="25" t="s">
-        <v>483</v>
-      </c>
-      <c r="I123" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="25">
-        <v>0.54237268518518522</v>
-      </c>
-      <c r="B124" t="s">
-        <v>415</v>
-      </c>
-      <c r="H124" s="25" t="s">
-        <v>484</v>
-      </c>
-      <c r="I124" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="25">
-        <v>0.54238425925925926</v>
-      </c>
-      <c r="B125" t="s">
-        <v>416</v>
-      </c>
-      <c r="H125" s="25" t="s">
-        <v>485</v>
-      </c>
-      <c r="I125" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="25">
-        <v>0.5423958333333333</v>
-      </c>
-      <c r="B126" t="s">
-        <v>417</v>
-      </c>
-      <c r="H126" s="25">
-        <v>13.2</v>
-      </c>
-      <c r="I126" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="25">
-        <v>13.2</v>
-      </c>
-      <c r="B127" t="s">
-        <v>418</v>
-      </c>
-      <c r="H127" s="25">
-        <v>13.3</v>
-      </c>
-      <c r="I127" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" s="25">
-        <v>13.3</v>
-      </c>
-      <c r="B128" t="s">
-        <v>419</v>
-      </c>
-      <c r="H128" s="25">
-        <v>13.4</v>
-      </c>
-      <c r="I128" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" s="25">
-        <v>13.4</v>
-      </c>
-      <c r="B129" t="s">
-        <v>420</v>
-      </c>
-      <c r="H129" s="25">
-        <v>14</v>
-      </c>
-      <c r="I129" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A130" s="25">
-        <v>14</v>
-      </c>
-      <c r="B130" t="s">
-        <v>421</v>
-      </c>
-      <c r="H130" s="25">
-        <v>15</v>
-      </c>
-      <c r="I130" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="25">
-        <v>15</v>
-      </c>
-      <c r="B131" t="s">
-        <v>422</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -6650,109 +4779,109 @@
       <c r="A1" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
@@ -6819,16 +4948,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7021,10 +5150,10 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="33"/>
+      <c r="G1" s="31"/>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Add in test for objectives and endpoints
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/simple_1.xlsx
+++ b/tests/integration_test_files/simple_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A259DC14-E722-E34F-B590-9D3E47CDAC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C096CFE3-C5C0-E141-AC29-6B069CB6D18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="6" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="5" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="560">
   <si>
     <t>Epoch</t>
   </si>
@@ -1729,18 +1729,36 @@
     <t/>
   </si>
   <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Primary Objectives</t>
+  </si>
+  <si>
     <r>
       <t>&lt;</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
       <t>usdm:ref klass="StudyIdentifier" id="StudyIdentifier_1" attribute="studyIdentifier"/&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;table&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top"&gt;Primary Objective&lt;/th&gt;
+    &lt;th style="vertical-align: top"&gt;Primary Endpoint&lt;/th&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Objective" id="Objective_1" attribute="description"/&gt;&lt;/td&gt;
+    &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Endpoint" id="Endpoint_1" attribute="description"/&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+&lt;/table&gt;</t>
   </si>
 </sst>
 </file>
@@ -1786,7 +1804,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Menlo"/>
       <family val="2"/>
@@ -1901,10 +1919,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2514,7 +2532,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3407,10 +3425,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3435,7 +3453,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
@@ -3444,7 +3462,7 @@
         <v>292</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3503,1114 +3521,1120 @@
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>430</v>
+    <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>556</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>295</v>
+        <v>557</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="B12" s="26"/>
+        <v>431</v>
+      </c>
       <c r="C12" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>511</v>
+        <v>435</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>489</v>
+        <v>512</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="10" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="10" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>485</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>478</v>
+        <v>517</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>518</v>
+        <v>481</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>490</v>
+        <v>518</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>519</v>
+        <v>490</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>436</v>
+        <v>521</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>522</v>
+        <v>436</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>437</v>
+        <v>523</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>524</v>
+        <v>439</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>440</v>
+        <v>524</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>487</v>
+        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>525</v>
+        <v>442</v>
       </c>
       <c r="B44" s="26"/>
       <c r="C44" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>443</v>
+        <v>526</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="10" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>491</v>
+        <v>446</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="10" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>527</v>
+        <v>491</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>447</v>
+        <v>527</v>
       </c>
       <c r="B52" s="26"/>
       <c r="C52" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="10" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B54" s="26"/>
       <c r="C54" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>529</v>
+        <v>449</v>
       </c>
       <c r="B55" s="26"/>
       <c r="C55" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B56" s="26"/>
       <c r="C56" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B57" s="26"/>
       <c r="C57" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>492</v>
+        <v>531</v>
       </c>
       <c r="B58" s="26"/>
       <c r="C58" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>532</v>
+        <v>492</v>
       </c>
       <c r="B59" s="26"/>
       <c r="C59" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B60" s="26"/>
       <c r="C60" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B61" s="26"/>
       <c r="C61" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>482</v>
+        <v>534</v>
       </c>
       <c r="B62" s="26"/>
       <c r="C62" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>450</v>
+        <v>482</v>
       </c>
       <c r="B63" s="26"/>
       <c r="C63" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B64" s="26"/>
       <c r="C64" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B65" s="26"/>
       <c r="C65" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B66" s="26"/>
       <c r="C66" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>535</v>
+        <v>453</v>
       </c>
       <c r="B67" s="26"/>
       <c r="C67" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>483</v>
+        <v>535</v>
       </c>
       <c r="B68" s="26"/>
       <c r="C68" s="10" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>454</v>
+        <v>483</v>
       </c>
       <c r="B69" s="26"/>
       <c r="C69" s="10" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B70" s="26"/>
       <c r="C70" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B71" s="26"/>
       <c r="C71" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B72" s="26"/>
       <c r="C72" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B73" s="26"/>
       <c r="C73" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B74" s="26"/>
       <c r="C74" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B75" s="26"/>
       <c r="C75" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B76" s="26"/>
       <c r="C76" s="10" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B77" s="26"/>
       <c r="C77" s="10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>536</v>
+        <v>462</v>
       </c>
       <c r="B78" s="26"/>
       <c r="C78" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>463</v>
+        <v>536</v>
       </c>
       <c r="B79" s="26"/>
       <c r="C79" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B80" s="26"/>
       <c r="C80" s="10" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>537</v>
+        <v>464</v>
       </c>
       <c r="B81" s="26"/>
       <c r="C81" s="10" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>465</v>
+        <v>537</v>
       </c>
       <c r="B82" s="26"/>
       <c r="C82" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B83" s="26"/>
       <c r="C83" s="10" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B84" s="26"/>
       <c r="C84" s="10" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B85" s="26"/>
       <c r="C85" s="10" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B86" s="26"/>
       <c r="C86" s="10" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>538</v>
+        <v>469</v>
       </c>
       <c r="B87" s="26"/>
       <c r="C87" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B88" s="26"/>
       <c r="C88" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B89" s="26"/>
       <c r="C89" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="B90" s="26"/>
       <c r="C90" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>484</v>
+        <v>532</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="B92" s="26"/>
       <c r="C92" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>541</v>
+        <v>493</v>
       </c>
       <c r="B93" s="26"/>
       <c r="C93" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B94" s="26"/>
       <c r="C94" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>470</v>
+        <v>542</v>
       </c>
       <c r="B95" s="26"/>
       <c r="C95" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B96" s="26"/>
       <c r="C96" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B97" s="26"/>
       <c r="C97" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B98" s="26"/>
       <c r="C98" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B99" s="26"/>
       <c r="C99" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>543</v>
+        <v>474</v>
       </c>
       <c r="B100" s="26"/>
       <c r="C100" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B101" s="26"/>
       <c r="C101" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B102" s="26"/>
       <c r="C102" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B103" s="26"/>
       <c r="C103" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B104" s="26"/>
       <c r="C104" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B105" s="26"/>
       <c r="C105" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B106" s="26"/>
       <c r="C106" s="10" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>494</v>
+        <v>549</v>
       </c>
       <c r="B107" s="26"/>
       <c r="C107" s="10" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>550</v>
+        <v>494</v>
       </c>
       <c r="B108" s="26"/>
       <c r="C108" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B109" s="26"/>
       <c r="C109" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B110" s="26"/>
       <c r="C110" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B111" s="26"/>
       <c r="C111" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B112" s="26"/>
       <c r="C112" s="10" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>495</v>
+        <v>554</v>
       </c>
       <c r="B113" s="26"/>
       <c r="C113" s="10" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="B114" s="26"/>
       <c r="C114" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B115" s="26"/>
       <c r="C115" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B116" s="26"/>
       <c r="C116" s="10" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="B117" s="26"/>
       <c r="C117" s="10" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="B118" s="26"/>
       <c r="C118" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B119" s="26"/>
       <c r="C119" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B120" s="26"/>
       <c r="C120" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B121" s="26"/>
       <c r="C121" s="10" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="B122" s="26"/>
       <c r="C122" s="10" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="B123" s="26"/>
       <c r="C123" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
-        <v>475</v>
+        <v>503</v>
       </c>
       <c r="B124" s="26"/>
       <c r="C124" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B125" s="26"/>
       <c r="C125" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B126" s="26"/>
       <c r="C126" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>502</v>
+        <v>477</v>
       </c>
       <c r="B127" s="26"/>
       <c r="C127" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B128" s="26"/>
       <c r="C128" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B129" s="26"/>
       <c r="C129" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B130" s="26"/>
       <c r="C130" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B131" s="26"/>
       <c r="C131" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="B132" s="26"/>
+      <c r="C132" s="10" t="s">
         <v>420</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="11" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -4635,6 +4659,11 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="11" t="s">
         <v>555</v>
       </c>
     </row>
@@ -4801,34 +4830,34 @@
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
@@ -4948,16 +4977,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Allow for name / xref references as well as id references
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/simple_1.xlsx
+++ b/tests/integration_test_files/simple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C096CFE3-C5C0-E141-AC29-6B069CB6D18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E64E4B-0DC5-1B42-8D4C-DCF74E850803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="5" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -1755,7 +1755,7 @@
     &lt;th style="vertical-align: top"&gt;Primary Endpoint&lt;/th&gt;
   &lt;/tr&gt;
   &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Objective" id="Objective_1" attribute="description"/&gt;&lt;/td&gt;
+    &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Objective" namexref="OBJ1" attribute="description"/&gt;&lt;/td&gt;
     &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Endpoint" id="Endpoint_1" attribute="description"/&gt;&lt;/td&gt;
   &lt;/tr&gt;
 &lt;/table&gt;</t>
@@ -2532,7 +2532,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update study sheet for new format
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/simple_1.xlsx
+++ b/tests/integration_test_files/simple_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E64E4B-0DC5-1B42-8D4C-DCF74E850803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A576F3A-688C-0C4F-9A0B-2DD550C52A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="5" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="87520" yWindow="4120" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="557">
   <si>
     <t>Epoch</t>
   </si>
@@ -506,12 +506,6 @@
     <t>protocolVersion</t>
   </si>
   <si>
-    <t>protocolAmendment</t>
-  </si>
-  <si>
-    <t>protocolEffectiveDate</t>
-  </si>
-  <si>
     <t>protocolStatus</t>
   </si>
   <si>
@@ -524,16 +518,10 @@
     <t>Something Public</t>
   </si>
   <si>
-    <t>Somethign Clever</t>
-  </si>
-  <si>
     <t>draft</t>
   </si>
   <si>
     <t>Somethign Clever But New</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>businessTherapeuticAreas</t>
@@ -1759,6 +1747,9 @@
     &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Endpoint" id="Endpoint_1" attribute="description"/&gt;&lt;/td&gt;
   &lt;/tr&gt;
 &lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>SIMPLE1</t>
   </si>
 </sst>
 </file>
@@ -1842,7 +1833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1880,9 +1871,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1897,9 +1885,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1919,10 +1904,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2241,286 +2226,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="16" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="17" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="B10" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="B11" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="B12" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="G9" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="B14" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="15">
-        <v>40179</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G11" s="15">
-        <v>40544</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3009,29 +2853,29 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
         <v>136</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F5" t="s">
         <v>114</v>
@@ -3040,7 +2884,7 @@
         <v>120</v>
       </c>
       <c r="H5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3071,63 +2915,63 @@
       <c r="A1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>191</v>
+      <c r="B1" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E3" t="s">
-        <v>196</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>197</v>
-      </c>
       <c r="G3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3159,138 +3003,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="G1" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>202</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3316,105 +3160,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>206</v>
+      <c r="B1" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3427,7 +3271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3440,1231 +3284,1231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
-        <v>528</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>488</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>290</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>291</v>
+      <c r="A1" s="25" t="s">
+        <v>524</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="10" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="B13" s="26"/>
+        <v>418</v>
+      </c>
+      <c r="B13" s="24"/>
       <c r="C13" s="10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>432</v>
-      </c>
-      <c r="B14" s="26"/>
+        <v>428</v>
+      </c>
+      <c r="B14" s="24"/>
       <c r="C14" s="10" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>433</v>
-      </c>
-      <c r="B15" s="26"/>
+        <v>429</v>
+      </c>
+      <c r="B15" s="24"/>
       <c r="C15" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>434</v>
-      </c>
-      <c r="B16" s="26"/>
+        <v>430</v>
+      </c>
+      <c r="B16" s="24"/>
       <c r="C16" s="10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>435</v>
-      </c>
-      <c r="B17" s="26"/>
+        <v>431</v>
+      </c>
+      <c r="B17" s="24"/>
       <c r="C17" s="10" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>511</v>
-      </c>
-      <c r="B18" s="26"/>
+        <v>507</v>
+      </c>
+      <c r="B18" s="24"/>
       <c r="C18" s="10" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>512</v>
-      </c>
-      <c r="B19" s="26"/>
+        <v>508</v>
+      </c>
+      <c r="B19" s="24"/>
       <c r="C19" s="10" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="B20" s="26"/>
+        <v>485</v>
+      </c>
+      <c r="B20" s="24"/>
       <c r="C20" s="10" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>513</v>
-      </c>
-      <c r="B21" s="26"/>
+        <v>509</v>
+      </c>
+      <c r="B21" s="24"/>
       <c r="C21" s="10" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>514</v>
-      </c>
-      <c r="B22" s="26"/>
+        <v>510</v>
+      </c>
+      <c r="B22" s="24"/>
       <c r="C22" s="10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>515</v>
-      </c>
-      <c r="B23" s="26"/>
+        <v>511</v>
+      </c>
+      <c r="B23" s="24"/>
       <c r="C23" s="10" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>516</v>
-      </c>
-      <c r="B24" s="26"/>
+        <v>512</v>
+      </c>
+      <c r="B24" s="24"/>
       <c r="C24" s="10" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="B25" s="26"/>
+        <v>513</v>
+      </c>
+      <c r="B25" s="24"/>
       <c r="C25" s="10" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>478</v>
-      </c>
-      <c r="B26" s="26"/>
+        <v>474</v>
+      </c>
+      <c r="B26" s="24"/>
       <c r="C26" s="10" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>479</v>
-      </c>
-      <c r="B27" s="26"/>
+        <v>475</v>
+      </c>
+      <c r="B27" s="24"/>
       <c r="C27" s="10" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>480</v>
-      </c>
-      <c r="B28" s="26"/>
+        <v>476</v>
+      </c>
+      <c r="B28" s="24"/>
       <c r="C28" s="10" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>481</v>
-      </c>
-      <c r="B29" s="26"/>
+        <v>477</v>
+      </c>
+      <c r="B29" s="24"/>
       <c r="C29" s="10" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>518</v>
-      </c>
-      <c r="B30" s="26"/>
+        <v>514</v>
+      </c>
+      <c r="B30" s="24"/>
       <c r="C30" s="10" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>490</v>
-      </c>
-      <c r="B31" s="26"/>
+        <v>486</v>
+      </c>
+      <c r="B31" s="24"/>
       <c r="C31" s="10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>519</v>
-      </c>
-      <c r="B32" s="26"/>
+        <v>515</v>
+      </c>
+      <c r="B32" s="24"/>
       <c r="C32" s="10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>520</v>
-      </c>
-      <c r="B33" s="26"/>
+        <v>516</v>
+      </c>
+      <c r="B33" s="24"/>
       <c r="C33" s="10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>521</v>
-      </c>
-      <c r="B34" s="26"/>
+        <v>517</v>
+      </c>
+      <c r="B34" s="24"/>
       <c r="C34" s="10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="B35" s="26"/>
+        <v>432</v>
+      </c>
+      <c r="B35" s="24"/>
       <c r="C35" s="10" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>522</v>
-      </c>
-      <c r="B36" s="26"/>
+        <v>518</v>
+      </c>
+      <c r="B36" s="24"/>
       <c r="C36" s="10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>523</v>
-      </c>
-      <c r="B37" s="26"/>
+        <v>519</v>
+      </c>
+      <c r="B37" s="24"/>
       <c r="C37" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>437</v>
-      </c>
-      <c r="B38" s="26"/>
+        <v>433</v>
+      </c>
+      <c r="B38" s="24"/>
       <c r="C38" s="10" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="B39" s="26"/>
+        <v>434</v>
+      </c>
+      <c r="B39" s="24"/>
       <c r="C39" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="B40" s="26"/>
+        <v>435</v>
+      </c>
+      <c r="B40" s="24"/>
       <c r="C40" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>524</v>
-      </c>
-      <c r="B41" s="26"/>
+        <v>520</v>
+      </c>
+      <c r="B41" s="24"/>
       <c r="C41" s="10" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>440</v>
-      </c>
-      <c r="B42" s="26"/>
+        <v>436</v>
+      </c>
+      <c r="B42" s="24"/>
       <c r="C42" s="10" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="B43" s="26"/>
+        <v>437</v>
+      </c>
+      <c r="B43" s="24"/>
       <c r="C43" s="10" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="B44" s="26"/>
+        <v>438</v>
+      </c>
+      <c r="B44" s="24"/>
       <c r="C44" s="10" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>525</v>
-      </c>
-      <c r="B45" s="26"/>
+        <v>521</v>
+      </c>
+      <c r="B45" s="24"/>
       <c r="C45" s="10" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>526</v>
-      </c>
-      <c r="B46" s="26"/>
+        <v>522</v>
+      </c>
+      <c r="B46" s="24"/>
       <c r="C46" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="B47" s="26"/>
+        <v>439</v>
+      </c>
+      <c r="B47" s="24"/>
       <c r="C47" s="10" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="B48" s="26"/>
+        <v>440</v>
+      </c>
+      <c r="B48" s="24"/>
       <c r="C48" s="10" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="B49" s="26"/>
+        <v>441</v>
+      </c>
+      <c r="B49" s="24"/>
       <c r="C49" s="10" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="B50" s="26"/>
+        <v>442</v>
+      </c>
+      <c r="B50" s="24"/>
       <c r="C50" s="10" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="B51" s="26"/>
+        <v>487</v>
+      </c>
+      <c r="B51" s="24"/>
       <c r="C51" s="10" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="B52" s="26"/>
+        <v>523</v>
+      </c>
+      <c r="B52" s="24"/>
       <c r="C52" s="10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="B53" s="26"/>
+        <v>443</v>
+      </c>
+      <c r="B53" s="24"/>
       <c r="C53" s="10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="B54" s="26"/>
+        <v>444</v>
+      </c>
+      <c r="B54" s="24"/>
       <c r="C54" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="B55" s="26"/>
+        <v>445</v>
+      </c>
+      <c r="B55" s="24"/>
       <c r="C55" s="10" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>529</v>
-      </c>
-      <c r="B56" s="26"/>
+        <v>525</v>
+      </c>
+      <c r="B56" s="24"/>
       <c r="C56" s="10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>530</v>
-      </c>
-      <c r="B57" s="26"/>
+        <v>526</v>
+      </c>
+      <c r="B57" s="24"/>
       <c r="C57" s="10" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>531</v>
-      </c>
-      <c r="B58" s="26"/>
+        <v>527</v>
+      </c>
+      <c r="B58" s="24"/>
       <c r="C58" s="10" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>492</v>
-      </c>
-      <c r="B59" s="26"/>
+        <v>488</v>
+      </c>
+      <c r="B59" s="24"/>
       <c r="C59" s="10" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>532</v>
-      </c>
-      <c r="B60" s="26"/>
+        <v>528</v>
+      </c>
+      <c r="B60" s="24"/>
       <c r="C60" s="10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="B61" s="26"/>
+        <v>529</v>
+      </c>
+      <c r="B61" s="24"/>
       <c r="C61" s="10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>534</v>
-      </c>
-      <c r="B62" s="26"/>
+        <v>530</v>
+      </c>
+      <c r="B62" s="24"/>
       <c r="C62" s="10" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>482</v>
-      </c>
-      <c r="B63" s="26"/>
+        <v>478</v>
+      </c>
+      <c r="B63" s="24"/>
       <c r="C63" s="10" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>450</v>
-      </c>
-      <c r="B64" s="26"/>
+        <v>446</v>
+      </c>
+      <c r="B64" s="24"/>
       <c r="C64" s="10" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="B65" s="26"/>
+        <v>447</v>
+      </c>
+      <c r="B65" s="24"/>
       <c r="C65" s="10" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="B66" s="26"/>
+        <v>448</v>
+      </c>
+      <c r="B66" s="24"/>
       <c r="C66" s="10" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="B67" s="26"/>
+        <v>449</v>
+      </c>
+      <c r="B67" s="24"/>
       <c r="C67" s="10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>535</v>
-      </c>
-      <c r="B68" s="26"/>
+        <v>531</v>
+      </c>
+      <c r="B68" s="24"/>
       <c r="C68" s="10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>483</v>
-      </c>
-      <c r="B69" s="26"/>
+        <v>479</v>
+      </c>
+      <c r="B69" s="24"/>
       <c r="C69" s="10" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>454</v>
-      </c>
-      <c r="B70" s="26"/>
+        <v>450</v>
+      </c>
+      <c r="B70" s="24"/>
       <c r="C70" s="10" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="B71" s="26"/>
+        <v>451</v>
+      </c>
+      <c r="B71" s="24"/>
       <c r="C71" s="10" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="B72" s="26"/>
+        <v>452</v>
+      </c>
+      <c r="B72" s="24"/>
       <c r="C72" s="10" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="B73" s="26"/>
+        <v>453</v>
+      </c>
+      <c r="B73" s="24"/>
       <c r="C73" s="10" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="B74" s="26"/>
+        <v>454</v>
+      </c>
+      <c r="B74" s="24"/>
       <c r="C74" s="10" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="B75" s="26"/>
+        <v>455</v>
+      </c>
+      <c r="B75" s="24"/>
       <c r="C75" s="10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="B76" s="26"/>
+        <v>456</v>
+      </c>
+      <c r="B76" s="24"/>
       <c r="C76" s="10" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="B77" s="26"/>
+        <v>457</v>
+      </c>
+      <c r="B77" s="24"/>
       <c r="C77" s="10" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="B78" s="26"/>
+        <v>458</v>
+      </c>
+      <c r="B78" s="24"/>
       <c r="C78" s="10" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>536</v>
-      </c>
-      <c r="B79" s="26"/>
+        <v>532</v>
+      </c>
+      <c r="B79" s="24"/>
       <c r="C79" s="10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="B80" s="26"/>
+        <v>459</v>
+      </c>
+      <c r="B80" s="24"/>
       <c r="C80" s="10" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>464</v>
-      </c>
-      <c r="B81" s="26"/>
+        <v>460</v>
+      </c>
+      <c r="B81" s="24"/>
       <c r="C81" s="10" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="B82" s="26"/>
+        <v>533</v>
+      </c>
+      <c r="B82" s="24"/>
       <c r="C82" s="10" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="B83" s="26"/>
+        <v>461</v>
+      </c>
+      <c r="B83" s="24"/>
       <c r="C83" s="10" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="B84" s="26"/>
+        <v>462</v>
+      </c>
+      <c r="B84" s="24"/>
       <c r="C84" s="10" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="B85" s="26"/>
+        <v>463</v>
+      </c>
+      <c r="B85" s="24"/>
       <c r="C85" s="10" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>468</v>
-      </c>
-      <c r="B86" s="26"/>
+        <v>464</v>
+      </c>
+      <c r="B86" s="24"/>
       <c r="C86" s="10" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="B87" s="26"/>
+        <v>465</v>
+      </c>
+      <c r="B87" s="24"/>
       <c r="C87" s="10" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>538</v>
-      </c>
-      <c r="B88" s="26"/>
+        <v>534</v>
+      </c>
+      <c r="B88" s="24"/>
       <c r="C88" s="10" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="B89" s="26"/>
+        <v>535</v>
+      </c>
+      <c r="B89" s="24"/>
       <c r="C89" s="10" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>540</v>
-      </c>
-      <c r="B90" s="26"/>
+        <v>536</v>
+      </c>
+      <c r="B90" s="24"/>
       <c r="C90" s="10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>532</v>
-      </c>
-      <c r="B91" s="26"/>
+        <v>528</v>
+      </c>
+      <c r="B91" s="24"/>
       <c r="C91" s="10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="B92" s="26"/>
+        <v>480</v>
+      </c>
+      <c r="B92" s="24"/>
       <c r="C92" s="10" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="B93" s="26"/>
+        <v>489</v>
+      </c>
+      <c r="B93" s="24"/>
       <c r="C93" s="10" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>541</v>
-      </c>
-      <c r="B94" s="26"/>
+        <v>537</v>
+      </c>
+      <c r="B94" s="24"/>
       <c r="C94" s="10" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>542</v>
-      </c>
-      <c r="B95" s="26"/>
+        <v>538</v>
+      </c>
+      <c r="B95" s="24"/>
       <c r="C95" s="10" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="B96" s="26"/>
+        <v>466</v>
+      </c>
+      <c r="B96" s="24"/>
       <c r="C96" s="10" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>471</v>
-      </c>
-      <c r="B97" s="26"/>
+        <v>467</v>
+      </c>
+      <c r="B97" s="24"/>
       <c r="C97" s="10" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="B98" s="26"/>
+        <v>468</v>
+      </c>
+      <c r="B98" s="24"/>
       <c r="C98" s="10" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>473</v>
-      </c>
-      <c r="B99" s="26"/>
+        <v>469</v>
+      </c>
+      <c r="B99" s="24"/>
       <c r="C99" s="10" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="B100" s="26"/>
+        <v>470</v>
+      </c>
+      <c r="B100" s="24"/>
       <c r="C100" s="10" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="B101" s="26"/>
+        <v>539</v>
+      </c>
+      <c r="B101" s="24"/>
       <c r="C101" s="10" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="B102" s="26"/>
+        <v>540</v>
+      </c>
+      <c r="B102" s="24"/>
       <c r="C102" s="10" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>545</v>
-      </c>
-      <c r="B103" s="26"/>
+        <v>541</v>
+      </c>
+      <c r="B103" s="24"/>
       <c r="C103" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>546</v>
-      </c>
-      <c r="B104" s="26"/>
+        <v>542</v>
+      </c>
+      <c r="B104" s="24"/>
       <c r="C104" s="10" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>547</v>
-      </c>
-      <c r="B105" s="26"/>
+        <v>543</v>
+      </c>
+      <c r="B105" s="24"/>
       <c r="C105" s="10" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>548</v>
-      </c>
-      <c r="B106" s="26"/>
+        <v>544</v>
+      </c>
+      <c r="B106" s="24"/>
       <c r="C106" s="10" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="B107" s="26"/>
+        <v>545</v>
+      </c>
+      <c r="B107" s="24"/>
       <c r="C107" s="10" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>494</v>
-      </c>
-      <c r="B108" s="26"/>
+        <v>490</v>
+      </c>
+      <c r="B108" s="24"/>
       <c r="C108" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>550</v>
-      </c>
-      <c r="B109" s="26"/>
+        <v>546</v>
+      </c>
+      <c r="B109" s="24"/>
       <c r="C109" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>551</v>
-      </c>
-      <c r="B110" s="26"/>
+        <v>547</v>
+      </c>
+      <c r="B110" s="24"/>
       <c r="C110" s="10" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>552</v>
-      </c>
-      <c r="B111" s="26"/>
+        <v>548</v>
+      </c>
+      <c r="B111" s="24"/>
       <c r="C111" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>553</v>
-      </c>
-      <c r="B112" s="26"/>
+        <v>549</v>
+      </c>
+      <c r="B112" s="24"/>
       <c r="C112" s="10" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>554</v>
-      </c>
-      <c r="B113" s="26"/>
+        <v>550</v>
+      </c>
+      <c r="B113" s="24"/>
       <c r="C113" s="10" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>495</v>
-      </c>
-      <c r="B114" s="26"/>
+        <v>491</v>
+      </c>
+      <c r="B114" s="24"/>
       <c r="C114" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>510</v>
-      </c>
-      <c r="B115" s="26"/>
+        <v>506</v>
+      </c>
+      <c r="B115" s="24"/>
       <c r="C115" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>509</v>
-      </c>
-      <c r="B116" s="26"/>
+        <v>505</v>
+      </c>
+      <c r="B116" s="24"/>
       <c r="C116" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>508</v>
-      </c>
-      <c r="B117" s="26"/>
+        <v>504</v>
+      </c>
+      <c r="B117" s="24"/>
       <c r="C117" s="10" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>496</v>
-      </c>
-      <c r="B118" s="26"/>
+        <v>492</v>
+      </c>
+      <c r="B118" s="24"/>
       <c r="C118" s="10" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="B119" s="26"/>
+        <v>503</v>
+      </c>
+      <c r="B119" s="24"/>
       <c r="C119" s="10" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>506</v>
-      </c>
-      <c r="B120" s="26"/>
+        <v>502</v>
+      </c>
+      <c r="B120" s="24"/>
       <c r="C120" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="B121" s="26"/>
+        <v>501</v>
+      </c>
+      <c r="B121" s="24"/>
       <c r="C121" s="10" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>504</v>
-      </c>
-      <c r="B122" s="26"/>
+        <v>500</v>
+      </c>
+      <c r="B122" s="24"/>
       <c r="C122" s="10" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>497</v>
-      </c>
-      <c r="B123" s="26"/>
+        <v>493</v>
+      </c>
+      <c r="B123" s="24"/>
       <c r="C123" s="10" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
-        <v>503</v>
-      </c>
-      <c r="B124" s="26"/>
+        <v>499</v>
+      </c>
+      <c r="B124" s="24"/>
       <c r="C124" s="10" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>475</v>
-      </c>
-      <c r="B125" s="26"/>
+        <v>471</v>
+      </c>
+      <c r="B125" s="24"/>
       <c r="C125" s="10" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>476</v>
-      </c>
-      <c r="B126" s="26"/>
+        <v>472</v>
+      </c>
+      <c r="B126" s="24"/>
       <c r="C126" s="10" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>477</v>
-      </c>
-      <c r="B127" s="26"/>
+        <v>473</v>
+      </c>
+      <c r="B127" s="24"/>
       <c r="C127" s="10" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="B128" s="26"/>
+        <v>498</v>
+      </c>
+      <c r="B128" s="24"/>
       <c r="C128" s="10" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>501</v>
-      </c>
-      <c r="B129" s="26"/>
+        <v>497</v>
+      </c>
+      <c r="B129" s="24"/>
       <c r="C129" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>500</v>
-      </c>
-      <c r="B130" s="26"/>
+        <v>496</v>
+      </c>
+      <c r="B130" s="24"/>
       <c r="C130" s="10" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>498</v>
-      </c>
-      <c r="B131" s="26"/>
+        <v>494</v>
+      </c>
+      <c r="B131" s="24"/>
       <c r="C131" s="10" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>499</v>
-      </c>
-      <c r="B132" s="26"/>
+        <v>495</v>
+      </c>
+      <c r="B132" s="24"/>
       <c r="C132" s="10" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -4688,18 +4532,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4725,22 +4569,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="21" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4755,7 +4599,7 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
@@ -4775,7 +4619,7 @@
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
@@ -4805,116 +4649,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="A1" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="B5" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="A9" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="A10" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>227</v>
+      <c r="A12" s="16" t="s">
+        <v>223</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>43</v>
@@ -4934,16 +4778,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -4951,16 +4795,16 @@
         <v>42</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4977,16 +4821,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5010,20 +4854,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>273</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -5031,16 +4875,16 @@
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5051,13 +4895,13 @@
         <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -5084,14 +4928,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>264</v>
+      <c r="A1" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5099,10 +4943,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5110,10 +4954,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -5121,10 +4965,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -5132,10 +4976,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -5164,13 +5008,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>182</v>
+      <c r="A1" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C1" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5179,22 +5023,22 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="A2" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -5214,13 +5058,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>186</v>
+      <c r="A3" s="16" t="s">
+        <v>182</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -5242,7 +5086,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -5264,7 +5108,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -5286,7 +5130,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -5308,30 +5152,30 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="17" t="s">
-        <v>224</v>
+      <c r="C7" s="16" t="s">
+        <v>220</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="17" t="s">
-        <v>225</v>
+      <c r="C8" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -5345,14 +5189,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>226</v>
+      <c r="C9" s="22" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5434,17 +5278,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>286</v>
+      <c r="A1" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5452,7 +5296,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5460,13 +5304,13 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>